<commit_message>
[Issues: #I9DN15] 新增 react-native-sensors 文档
</commit_message>
<xml_diff>
--- a/Menu.xlsx
+++ b/Menu.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25800" windowHeight="12820"/>
+    <workbookView windowWidth="28800" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="303">
   <si>
     <t>序号</t>
   </si>
@@ -930,6 +930,15 @@
   </si>
   <si>
     <t>5.1.5</t>
+  </si>
+  <si>
+    <t>reatc-native-sensors</t>
+  </si>
+  <si>
+    <t>7.2.1</t>
+  </si>
+  <si>
+    <t>@react-native-oh-library/react-native-sensors</t>
   </si>
 </sst>
 </file>
@@ -2131,23 +2140,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F122"/>
+  <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="G104" sqref="G104"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="G121" sqref="G121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="13.9423076923077" style="1" customWidth="1"/>
-    <col min="2" max="2" width="52.7307692307692" style="1" customWidth="1"/>
-    <col min="3" max="4" width="9.23076923076923" style="1"/>
-    <col min="5" max="5" width="51.9230769230769" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.3365384615385" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.23076923076923" style="1"/>
+    <col min="1" max="1" width="13.9416666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.7333333333333" style="1" customWidth="1"/>
+    <col min="3" max="4" width="9.23333333333333" style="1"/>
+    <col min="5" max="5" width="51.925" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.3333333333333" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.23333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="51.75" spans="1:6">
+    <row r="1" ht="41.25" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2167,7 +2176,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="17.75" spans="1:6">
+    <row r="2" ht="14.25" spans="1:6">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2187,7 +2196,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" ht="17.75" spans="1:6">
+    <row r="3" ht="14.25" spans="1:6">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2207,7 +2216,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" ht="17.75" spans="1:6">
+    <row r="4" ht="14.25" spans="1:6">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2227,7 +2236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" ht="17.75" spans="1:6">
+    <row r="5" ht="14.25" spans="1:6">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2247,7 +2256,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" ht="17.75" spans="1:6">
+    <row r="6" ht="14.25" spans="1:6">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2267,7 +2276,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" ht="17.75" spans="1:6">
+    <row r="7" ht="14.25" spans="1:6">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2287,7 +2296,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" ht="17.75" spans="1:6">
+    <row r="8" ht="14.25" spans="1:6">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2307,7 +2316,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" ht="17.75" spans="1:6">
+    <row r="9" ht="14.25" spans="1:6">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2327,7 +2336,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" ht="17.75" spans="1:6">
+    <row r="10" ht="14.25" spans="1:6">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2347,7 +2356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" ht="17.75" spans="1:6">
+    <row r="11" ht="14.25" spans="1:6">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2367,7 +2376,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" ht="17.75" spans="1:6">
+    <row r="12" ht="14.25" spans="1:6">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2387,7 +2396,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" ht="17.75" spans="1:6">
+    <row r="13" ht="14.25" spans="1:6">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2407,7 +2416,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" ht="17.75" spans="1:6">
+    <row r="14" ht="14.25" spans="1:6">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2427,7 +2436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" ht="17.75" spans="1:6">
+    <row r="15" ht="14.25" spans="1:6">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2447,7 +2456,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" ht="17.75" spans="1:6">
+    <row r="16" ht="14.25" spans="1:6">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2467,7 +2476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" ht="17.75" spans="1:6">
+    <row r="17" ht="14.25" spans="1:6">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2487,7 +2496,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" ht="17.75" spans="1:6">
+    <row r="18" ht="14.25" spans="1:6">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2507,7 +2516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" ht="17.75" spans="1:6">
+    <row r="19" ht="14.25" spans="1:6">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2527,7 +2536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" ht="17.75" spans="1:6">
+    <row r="20" ht="14.25" spans="1:6">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2547,7 +2556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" ht="17.75" spans="1:6">
+    <row r="21" ht="14.25" spans="1:6">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2567,7 +2576,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" ht="17.75" spans="1:6">
+    <row r="22" ht="14.25" spans="1:6">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2587,7 +2596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" ht="17.75" spans="1:6">
+    <row r="23" ht="14.25" spans="1:6">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2607,7 +2616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" ht="17.75" spans="1:6">
+    <row r="24" ht="14.25" spans="1:6">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2627,7 +2636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" ht="17.75" spans="1:6">
+    <row r="25" ht="14.25" spans="1:6">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2647,7 +2656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" ht="17.75" spans="1:6">
+    <row r="26" ht="14.25" spans="1:6">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2667,7 +2676,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" ht="17.75" spans="1:6">
+    <row r="27" ht="14.25" spans="1:6">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2687,7 +2696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" ht="17.75" spans="1:6">
+    <row r="28" ht="14.25" spans="1:6">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2707,7 +2716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" ht="17.75" spans="1:6">
+    <row r="29" ht="14.25" spans="1:6">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2727,7 +2736,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" ht="17.75" spans="1:6">
+    <row r="30" ht="14.25" spans="1:6">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2747,7 +2756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" ht="17.75" spans="1:6">
+    <row r="31" ht="14.25" spans="1:6">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2767,7 +2776,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" ht="17.75" spans="1:6">
+    <row r="32" ht="14.25" spans="1:6">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2787,7 +2796,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" ht="17.75" spans="1:6">
+    <row r="33" ht="14.25" spans="1:6">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2807,7 +2816,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" ht="17.75" spans="1:6">
+    <row r="34" ht="14.25" spans="1:6">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2827,7 +2836,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" ht="17.75" spans="1:6">
+    <row r="35" ht="14.25" spans="1:6">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2847,7 +2856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" ht="17.75" spans="1:6">
+    <row r="36" ht="14.25" spans="1:6">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -2867,7 +2876,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" ht="17.75" spans="1:6">
+    <row r="37" ht="14.25" spans="1:6">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -2887,7 +2896,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" ht="17.75" spans="1:6">
+    <row r="38" ht="14.25" spans="1:6">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -2907,7 +2916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" ht="17.75" spans="1:6">
+    <row r="39" ht="14.25" spans="1:6">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -2927,7 +2936,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" ht="17.75" spans="1:6">
+    <row r="40" ht="14.25" spans="1:6">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -2947,7 +2956,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" ht="17.75" spans="1:6">
+    <row r="41" ht="14.25" spans="1:6">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -2967,7 +2976,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" ht="17.75" spans="1:6">
+    <row r="42" ht="14.25" spans="1:6">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -2987,7 +2996,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" ht="17.75" spans="1:6">
+    <row r="43" ht="14.25" spans="1:6">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -3007,7 +3016,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" ht="17.75" spans="1:6">
+    <row r="44" ht="14.25" spans="1:6">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -3027,7 +3036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" ht="17.75" spans="1:6">
+    <row r="45" ht="14.25" spans="1:6">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -3047,7 +3056,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" ht="17.75" spans="1:6">
+    <row r="46" ht="14.25" spans="1:6">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -3067,7 +3076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" ht="17.75" spans="1:6">
+    <row r="47" ht="14.25" spans="1:6">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -3087,7 +3096,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" ht="17.75" spans="1:6">
+    <row r="48" ht="14.25" spans="1:6">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -3107,7 +3116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" ht="17.75" spans="1:6">
+    <row r="49" ht="27.75" spans="1:6">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -3127,7 +3136,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" ht="17.75" spans="1:6">
+    <row r="50" ht="14.25" spans="1:6">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -3147,7 +3156,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" ht="17.75" spans="1:6">
+    <row r="51" ht="14.25" spans="1:6">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -3167,7 +3176,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" ht="17.75" spans="1:6">
+    <row r="52" ht="14.25" spans="1:6">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -3187,7 +3196,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" ht="17.75" spans="1:6">
+    <row r="53" ht="14.25" spans="1:6">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -3207,7 +3216,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" ht="17.75" spans="1:6">
+    <row r="54" ht="14.25" spans="1:6">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -3227,7 +3236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" ht="17.75" spans="1:6">
+    <row r="55" ht="14.25" spans="1:6">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -3247,7 +3256,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" ht="17.75" spans="1:6">
+    <row r="56" ht="14.25" spans="1:6">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -3267,7 +3276,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" ht="17.75" spans="1:6">
+    <row r="57" ht="14.25" spans="1:6">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -3287,7 +3296,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" ht="17.75" spans="1:6">
+    <row r="58" ht="14.25" spans="1:6">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -3307,7 +3316,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" ht="17.75" spans="1:6">
+    <row r="59" ht="14.25" spans="1:6">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -3327,7 +3336,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" ht="17.75" spans="1:6">
+    <row r="60" ht="14.25" spans="1:6">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -3347,7 +3356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" ht="17.75" spans="1:6">
+    <row r="61" ht="14.25" spans="1:6">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -3367,7 +3376,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" ht="17.75" spans="1:6">
+    <row r="62" ht="14.25" spans="1:6">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -3387,7 +3396,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" ht="17.75" spans="1:6">
+    <row r="63" ht="14.25" spans="1:6">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -3407,7 +3416,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" ht="17.75" spans="1:6">
+    <row r="64" ht="14.25" spans="1:6">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -3427,7 +3436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" ht="17.75" spans="1:6">
+    <row r="65" ht="14.25" spans="1:6">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -3447,7 +3456,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" ht="17.75" spans="1:6">
+    <row r="66" ht="14.25" spans="1:6">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -3467,7 +3476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" ht="17.75" spans="1:6">
+    <row r="67" ht="14.25" spans="1:6">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -3487,7 +3496,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" ht="17.75" spans="1:6">
+    <row r="68" ht="14.25" spans="1:6">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -3505,7 +3514,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" ht="17.75" spans="1:6">
+    <row r="69" ht="14.25" spans="1:6">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -3525,7 +3534,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" ht="17.75" spans="1:6">
+    <row r="70" ht="27.75" spans="1:6">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -3545,7 +3554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" ht="34.75" spans="1:6">
+    <row r="71" ht="27.75" spans="1:6">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -3565,7 +3574,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" ht="34.75" spans="1:6">
+    <row r="72" ht="27.75" spans="1:6">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -3585,7 +3594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" ht="17.75" spans="1:6">
+    <row r="73" ht="14.25" spans="1:6">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -3605,7 +3614,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" ht="17.75" spans="1:6">
+    <row r="74" ht="14.25" spans="1:6">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -3625,7 +3634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" ht="17.75" spans="1:6">
+    <row r="75" ht="14.25" spans="1:6">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -3645,7 +3654,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" ht="17.75" spans="1:6">
+    <row r="76" ht="14.25" spans="1:6">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -3665,7 +3674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" ht="17.75" spans="1:6">
+    <row r="77" ht="14.25" spans="1:6">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -3685,7 +3694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" ht="17.75" spans="1:6">
+    <row r="78" ht="14.25" spans="1:6">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -3705,7 +3714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" ht="17.75" spans="1:6">
+    <row r="79" ht="14.25" spans="1:6">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -3725,7 +3734,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" ht="17.75" spans="1:6">
+    <row r="80" ht="14.25" spans="1:6">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -3745,7 +3754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" ht="17.75" spans="1:6">
+    <row r="81" ht="14.25" spans="1:6">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -3765,7 +3774,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" ht="17.75" spans="1:6">
+    <row r="82" ht="14.25" spans="1:6">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -3785,7 +3794,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" ht="17.75" spans="1:6">
+    <row r="83" ht="14.25" spans="1:6">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -3805,7 +3814,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" ht="17.75" spans="1:6">
+    <row r="84" ht="14.25" spans="1:6">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -3825,7 +3834,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" ht="17.75" spans="1:6">
+    <row r="85" ht="14.25" spans="1:6">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -3845,7 +3854,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" ht="17.75" spans="1:6">
+    <row r="86" ht="14.25" spans="1:6">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -3865,7 +3874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" ht="17.75" spans="1:6">
+    <row r="87" ht="14.25" spans="1:6">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -3885,7 +3894,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" ht="17.75" spans="1:6">
+    <row r="88" ht="14.25" spans="1:6">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -3905,7 +3914,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" ht="17.75" spans="1:6">
+    <row r="89" ht="14.25" spans="1:6">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -3925,7 +3934,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" ht="17.75" spans="1:6">
+    <row r="90" ht="14.25" spans="1:6">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -3945,7 +3954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" ht="17.75" spans="1:6">
+    <row r="91" ht="14.25" spans="1:6">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -3965,7 +3974,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" ht="17.75" spans="1:6">
+    <row r="92" ht="27.75" spans="1:6">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -3985,7 +3994,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" ht="17.75" spans="1:6">
+    <row r="93" ht="14.25" spans="1:6">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -4005,7 +4014,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" ht="17.75" spans="1:6">
+    <row r="94" ht="27.75" spans="1:6">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -4025,7 +4034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" ht="17.75" spans="1:6">
+    <row r="95" ht="14.25" spans="1:6">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -4045,7 +4054,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" ht="17.75" spans="1:6">
+    <row r="96" ht="14.25" spans="1:6">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -4065,7 +4074,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" ht="17.75" spans="1:6">
+    <row r="97" ht="14.25" spans="1:6">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -4085,7 +4094,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" ht="17.75" spans="1:6">
+    <row r="98" ht="14.25" spans="1:6">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -4105,7 +4114,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" ht="17.75" spans="1:6">
+    <row r="99" ht="14.25" spans="1:6">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -4125,7 +4134,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" ht="17.75" spans="1:6">
+    <row r="100" ht="14.25" spans="1:6">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -4145,7 +4154,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" ht="17.75" spans="1:6">
+    <row r="101" ht="14.25" spans="1:6">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -4165,7 +4174,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" ht="17.75" spans="1:6">
+    <row r="102" ht="14.25" spans="1:6">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -4185,7 +4194,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" ht="17.75" spans="1:6">
+    <row r="103" ht="14.25" spans="1:6">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -4205,7 +4214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" ht="17.75" spans="1:6">
+    <row r="104" ht="14.25" spans="1:6">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -4225,7 +4234,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" ht="17.75" spans="1:6">
+    <row r="105" ht="14.25" spans="1:6">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -4245,7 +4254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" ht="17.75" spans="1:6">
+    <row r="106" ht="14.25" spans="1:6">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -4265,7 +4274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" ht="17.75" spans="1:6">
+    <row r="107" ht="14.25" spans="1:6">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -4285,7 +4294,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" ht="17.75" spans="1:6">
+    <row r="108" spans="1:6">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -4305,7 +4314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" ht="17.75" spans="1:6">
+    <row r="109" ht="14.25" spans="1:6">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -4325,7 +4334,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" ht="17.75" spans="1:6">
+    <row r="110" ht="14.25" spans="1:6">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -4345,7 +4354,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" ht="17.75" spans="1:6">
+    <row r="111" ht="14.25" spans="1:6">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -4365,7 +4374,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" ht="17.75" spans="1:6">
+    <row r="112" ht="14.25" spans="1:6">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -4385,7 +4394,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" ht="17.75" spans="1:6">
+    <row r="113" ht="14.25" spans="1:6">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -4405,7 +4414,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114" ht="17.75" spans="1:6">
+    <row r="114" ht="14.25" spans="1:6">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -4425,7 +4434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" ht="17.75" spans="1:6">
+    <row r="115" ht="14.25" spans="1:6">
       <c r="A115" s="3">
         <v>114</v>
       </c>
@@ -4445,7 +4454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" ht="17.75" spans="1:6">
+    <row r="116" ht="14.25" spans="1:6">
       <c r="A116" s="3">
         <v>115</v>
       </c>
@@ -4465,7 +4474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117" ht="17.75" spans="1:6">
+    <row r="117" ht="14.25" spans="1:6">
       <c r="A117" s="3">
         <v>116</v>
       </c>
@@ -4485,7 +4494,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" ht="17.75" spans="1:6">
+    <row r="118" ht="14.25" spans="1:6">
       <c r="A118" s="3">
         <v>117</v>
       </c>
@@ -4505,7 +4514,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="119" ht="17.75" spans="1:6">
+    <row r="119" ht="14.25" spans="1:6">
       <c r="A119" s="3">
         <v>118</v>
       </c>
@@ -4525,7 +4534,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" ht="17.75" spans="1:6">
+    <row r="120" ht="14.25" spans="1:6">
       <c r="A120" s="3">
         <v>119</v>
       </c>
@@ -4545,7 +4554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="121" ht="17.75" spans="1:6">
+    <row r="121" ht="14.25" spans="1:6">
       <c r="A121" s="3">
         <v>120</v>
       </c>
@@ -4565,7 +4574,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" ht="17.75" spans="1:6">
+    <row r="122" ht="14.25" spans="1:6">
       <c r="A122" s="3">
         <v>121</v>
       </c>
@@ -4582,6 +4591,26 @@
         <v>59</v>
       </c>
       <c r="F122" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="123" ht="14.25" spans="1:6">
+      <c r="A123" s="3">
+        <v>122</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E123" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="F123" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4893,6 +4922,7 @@
     <hyperlink ref="E92" r:id="rId179" display="@react-native-oh-tpl/react-native-scrollable-tab-view" tooltip="https://github.com/react-native-oh-library/react-native-scrollable-tab-view/releases"/>
     <hyperlink ref="F55" r:id="rId3" location="/zh-cn/react-native-crypto-js" display="链接"/>
     <hyperlink ref="F76" r:id="rId3" location="/zh-cn/react-native-MJRefresh" display="链接"/>
+    <hyperlink ref="F123" r:id="rId3" location="/zh-cn/react-native-sensors" display="链接"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
!507 [Issues: #I9KZEP] 新增 react-navigation-native-stack 文档 * [Issues: #I9KZEP] 新增 react-navigation-native-stack 文档
</commit_message>
<xml_diff>
--- a/Menu.xlsx
+++ b/Menu.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="11175"/>
+    <workbookView windowWidth="28800" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="317">
   <si>
     <t>序号</t>
   </si>
@@ -969,6 +969,18 @@
   </si>
   <si>
     <t>1.1.2</t>
+  </si>
+  <si>
+    <t>@react-navigation/native-stack</t>
+  </si>
+  <si>
+    <t>6.9.26</t>
+  </si>
+  <si>
+    <t>−</t>
+  </si>
+  <si>
+    <t>@react-native-oh-tpl/native-stack</t>
   </si>
 </sst>
 </file>
@@ -981,7 +993,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1019,6 +1031,12 @@
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1505,128 +1523,128 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1648,10 +1666,13 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2179,10 +2200,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F127"/>
+  <dimension ref="A1:F128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="B131" sqref="B131"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="G128" sqref="G128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -4633,7 +4654,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" ht="14.25" spans="1:6">
+    <row r="123" spans="1:6">
       <c r="A123" s="3">
         <v>122</v>
       </c>
@@ -4653,7 +4674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" ht="14.25" spans="1:6">
+    <row r="124" spans="1:6">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -4669,7 +4690,7 @@
       <c r="E124" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="F124" s="8" t="s">
+      <c r="F124" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4677,7 +4698,7 @@
       <c r="A125" s="1">
         <v>124</v>
       </c>
-      <c r="B125" s="7" t="s">
+      <c r="B125" s="8" t="s">
         <v>306</v>
       </c>
       <c r="C125" s="1" t="s">
@@ -4689,7 +4710,7 @@
       <c r="E125" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F125" s="7" t="s">
+      <c r="F125" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4697,7 +4718,7 @@
       <c r="A126" s="1">
         <v>125</v>
       </c>
-      <c r="B126" s="7" t="s">
+      <c r="B126" s="8" t="s">
         <v>308</v>
       </c>
       <c r="C126" s="1" t="s">
@@ -4706,10 +4727,10 @@
       <c r="D126" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E126" s="7" t="s">
+      <c r="E126" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="F126" s="7" t="s">
+      <c r="F126" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4717,7 +4738,7 @@
       <c r="A127" s="1">
         <v>126</v>
       </c>
-      <c r="B127" s="7" t="s">
+      <c r="B127" s="8" t="s">
         <v>311</v>
       </c>
       <c r="C127" s="1" t="s">
@@ -4730,6 +4751,26 @@
         <v>59</v>
       </c>
       <c r="F127" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="128" ht="14.25" spans="1:6">
+      <c r="A128" s="1">
+        <v>127</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D128" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E128" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="F128" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -5054,6 +5095,9 @@
     <hyperlink ref="F127" r:id="rId3" location="/zh-cn/react-native-feather" display="链接"/>
     <hyperlink ref="B125" r:id="rId193" display="react-native-easy-toast"/>
     <hyperlink ref="F125" r:id="rId3" location="/zh-cn/react-native-sequence-2" display="链接"/>
+    <hyperlink ref="B128" r:id="rId194" display="@react-navigation/native-stack"/>
+    <hyperlink ref="E128" r:id="rId195" display="@react-native-oh-tpl/native-stack"/>
+    <hyperlink ref="F128" r:id="rId3" location="/zh-cn/react-navigation-native-stack.md" display="链接"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
docs: [Issues: #I9S3Y2] 添加文档总览内容
</commit_message>
<xml_diff>
--- a/Menu.xlsx
+++ b/Menu.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="337">
   <si>
     <t>序号</t>
   </si>
@@ -981,6 +981,66 @@
   </si>
   <si>
     <t>@react-native-oh-tpl/native-stack</t>
+  </si>
+  <si>
+    <t>react-native-waterfall-flow</t>
+  </si>
+  <si>
+    <t>1.1.5</t>
+  </si>
+  <si>
+    <t>react-native-vconsole</t>
+  </si>
+  <si>
+    <t>0.1.11</t>
+  </si>
+  <si>
+    <t>better-banner</t>
+  </si>
+  <si>
+    <t>0.0.1</t>
+  </si>
+  <si>
+    <t>react-native-ezswiper</t>
+  </si>
+  <si>
+    <t>1.3.0</t>
+  </si>
+  <si>
+    <t>react-native-image-header-scroll-view</t>
+  </si>
+  <si>
+    <t>0.10.3</t>
+  </si>
+  <si>
+    <t>react-native-linear-gradient-text</t>
+  </si>
+  <si>
+    <t>1.2.8</t>
+  </si>
+  <si>
+    <t>react-native-marquee-ab</t>
+  </si>
+  <si>
+    <t>2.0.0-rc.1</t>
+  </si>
+  <si>
+    <t>react-native-reconnecting-websocket</t>
+  </si>
+  <si>
+    <t>1.0.3</t>
+  </si>
+  <si>
+    <t>react-native-json-tree</t>
+  </si>
+  <si>
+    <t>react-native-image-gallery</t>
+  </si>
+  <si>
+    <t>2.1.5</t>
+  </si>
+  <si>
+    <t>@react-native-oh-tpl/react-native-image-gallery</t>
   </si>
 </sst>
 </file>
@@ -2200,10 +2260,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F128"/>
+  <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="G128" sqref="G128"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="I111" sqref="I111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -2236,7 +2296,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="14.25" spans="1:6">
+    <row r="2" spans="1:6">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -4654,7 +4714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" ht="14.25" spans="1:6">
       <c r="A123" s="3">
         <v>122</v>
       </c>
@@ -4674,7 +4734,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" ht="14.25" spans="1:6">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -4773,6 +4833,209 @@
       <c r="F128" s="8" t="s">
         <v>10</v>
       </c>
+    </row>
+    <row r="129" ht="14.25" spans="1:6">
+      <c r="A129" s="1">
+        <v>128</v>
+      </c>
+      <c r="B129" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D129" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E129" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="F129" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130" ht="14.25" spans="1:6">
+      <c r="A130" s="1">
+        <v>129</v>
+      </c>
+      <c r="B130" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D130" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E130" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="F130" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" ht="14.25" spans="1:6">
+      <c r="A131" s="1">
+        <v>130</v>
+      </c>
+      <c r="B131" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D131" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E131" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="F131" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" ht="14.25" spans="1:6">
+      <c r="A132" s="1">
+        <v>131</v>
+      </c>
+      <c r="B132" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D132" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E132" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="F132" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" ht="14.25" spans="1:6">
+      <c r="A133" s="1">
+        <v>132</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D133" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E133" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="F133" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" ht="14.25" spans="1:6">
+      <c r="A134" s="1">
+        <v>133</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D134" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E134" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="F134" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="135" ht="14.25" spans="1:6">
+      <c r="A135" s="1">
+        <v>134</v>
+      </c>
+      <c r="B135" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D135" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E135" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="F135" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" ht="14.25" spans="1:6">
+      <c r="A136" s="1">
+        <v>135</v>
+      </c>
+      <c r="B136" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D136" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E136" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="F136" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="137" ht="14.25" spans="1:6">
+      <c r="A137" s="1">
+        <v>136</v>
+      </c>
+      <c r="B137" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D137" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E137" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="F137" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="138" ht="14.25" spans="1:6">
+      <c r="A138" s="1">
+        <v>137</v>
+      </c>
+      <c r="B138" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D138" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E138" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F138" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" ht="14.25" spans="2:2">
+      <c r="B139" s="9"/>
     </row>
   </sheetData>
   <sortState ref="A2:F122">
@@ -4918,186 +5181,207 @@
     <hyperlink ref="F120" r:id="rId85" display="链接"/>
     <hyperlink ref="B121" r:id="rId86" display="styled-components" tooltip="https://github.com/styled-components/styled-components"/>
     <hyperlink ref="F121" r:id="rId87" display="链接"/>
-    <hyperlink ref="B122" r:id="rId12" display="styled-system" tooltip="https://github.com/react-native-picker/picker"/>
-    <hyperlink ref="F122" r:id="rId88" display="链接"/>
-    <hyperlink ref="B31" r:id="rId89" display="jeanregisser/react-native-slider" tooltip="https://github.com/react-native-oh-library/jeanregisser-react-native-slider"/>
+    <hyperlink ref="B122" r:id="rId88" display="styled-system" tooltip="https://github.com/react-native-picker/picker"/>
+    <hyperlink ref="F122" r:id="rId89" display="链接"/>
+    <hyperlink ref="B31" r:id="rId90" display="jeanregisser/react-native-slider" tooltip="https://github.com/react-native-oh-library/jeanregisser-react-native-slider"/>
     <hyperlink ref="F31" r:id="rId3" location="/zh-cn/jeanregisser-react-native-slider" display="链接"/>
     <hyperlink ref="B34" r:id="rId53" display="js-beautify" tooltip="https://github.com/beautifier/js-beautify"/>
     <hyperlink ref="F34" r:id="rId3" location="/zh-cn/js-beautify" display="链接"/>
-    <hyperlink ref="B50" r:id="rId90" display="react-native-base64" tooltip="https://github.com/eranbo/react-native-base64"/>
+    <hyperlink ref="B50" r:id="rId91" display="react-native-base64" tooltip="https://github.com/eranbo/react-native-base64"/>
     <hyperlink ref="F50" r:id="rId3" location="/zh-cn/react-native-base64" display="链接"/>
-    <hyperlink ref="B53" r:id="rId91" display="react-native-check-box" tooltip="https://github.com/crazycodeboy/react-native-check-box"/>
+    <hyperlink ref="B53" r:id="rId92" display="react-native-check-box" tooltip="https://github.com/crazycodeboy/react-native-check-box"/>
     <hyperlink ref="F53" r:id="rId3" location="/zh-cn/react-native-check-box" display="链接"/>
-    <hyperlink ref="B5" r:id="rId92" display="@react-native-community/blur" tooltip="https://github.com/Kureev/react-native-blur"/>
-    <hyperlink ref="E5" r:id="rId93" display="@react-native-oh-tpl/blur Releases" tooltip="https://github.com/react-native-oh-library/react-native-blur/releases"/>
+    <hyperlink ref="B5" r:id="rId93" display="@react-native-community/blur" tooltip="https://github.com/Kureev/react-native-blur"/>
+    <hyperlink ref="E5" r:id="rId94" display="@react-native-oh-tpl/blur Releases" tooltip="https://github.com/react-native-oh-library/react-native-blur/releases"/>
     <hyperlink ref="F5" r:id="rId3" location="/zh-cn/react-native-community-blur" display="链接"/>
-    <hyperlink ref="B12" r:id="rId94" display="@react-native-community/push-notification-ios" tooltip="https://github.com/react-native-push-notification/ios"/>
-    <hyperlink ref="E12" r:id="rId95" display="@react-native-oh-tpl/push-notification-ios" tooltip="https://github.com/react-native-oh-library/react-native-push-notification-ios/releases"/>
+    <hyperlink ref="B12" r:id="rId95" display="@react-native-community/push-notification-ios" tooltip="https://github.com/react-native-push-notification/ios"/>
+    <hyperlink ref="E12" r:id="rId96" display="@react-native-oh-tpl/push-notification-ios" tooltip="https://github.com/react-native-oh-library/react-native-push-notification-ios/releases"/>
     <hyperlink ref="F12" r:id="rId3" location="/zh-cn/react-native-community-push-notification-ios" display="链接"/>
-    <hyperlink ref="B15" r:id="rId96" display="@react-native-cookies/cookies" tooltip="https://github.com/react-native-cookies/cookies"/>
-    <hyperlink ref="E15" r:id="rId97" display="@react-native-oh-tpl/cookies" tooltip="https://github.com/react-native-oh-library/react-native-cookies/releases"/>
+    <hyperlink ref="B15" r:id="rId97" display="@react-native-cookies/cookies" tooltip="https://github.com/react-native-cookies/cookies"/>
+    <hyperlink ref="E15" r:id="rId98" display="@react-native-oh-tpl/cookies" tooltip="https://github.com/react-native-oh-library/react-native-cookies/releases"/>
     <hyperlink ref="F15" r:id="rId3" location="/zh-cn/react-native-cookies" display="链接"/>
-    <hyperlink ref="B55" r:id="rId98" display="react-native-crypto-js" tooltip="https://github.com/imchintan/react-native-crypto-js"/>
-    <hyperlink ref="B73" r:id="rId99" display="react-native-maps" tooltip="https://github.com/react-native-maps/react-native-maps"/>
-    <hyperlink ref="E73" r:id="rId100" display="@react-native-oh-tpl/react-native-maps" tooltip="https://github.com/react-native-maps/react-native-maps/releases"/>
+    <hyperlink ref="B55" r:id="rId99" display="react-native-crypto-js" tooltip="https://github.com/imchintan/react-native-crypto-js"/>
+    <hyperlink ref="B73" r:id="rId100" display="react-native-maps" tooltip="https://github.com/react-native-maps/react-native-maps"/>
+    <hyperlink ref="E73" r:id="rId101" display="@react-native-oh-tpl/react-native-maps" tooltip="https://github.com/react-native-maps/react-native-maps/releases"/>
     <hyperlink ref="F73" r:id="rId3" location="/zh-cn/react-native-maps" display="链接"/>
-    <hyperlink ref="B78" r:id="rId101" display="react-native-pdf" tooltip="https://github.com/wonday/react-native-pdf"/>
-    <hyperlink ref="E78" r:id="rId102" display="@react-native-oh-tpl/react-native-pdf" tooltip="https://github.com/react-native-oh-library/react-native-pdf/releases"/>
+    <hyperlink ref="B78" r:id="rId102" display="react-native-pdf" tooltip="https://github.com/wonday/react-native-pdf"/>
+    <hyperlink ref="E78" r:id="rId103" display="@react-native-oh-tpl/react-native-pdf" tooltip="https://github.com/react-native-oh-library/react-native-pdf/releases"/>
     <hyperlink ref="F78" r:id="rId3" location="/zh-cn/react-native-pdf" display="链接"/>
-    <hyperlink ref="B88" r:id="rId103" display="react-native-redash" tooltip="https://github.com/wcandillon/react-native-redash/"/>
+    <hyperlink ref="B88" r:id="rId104" display="react-native-redash" tooltip="https://github.com/wcandillon/react-native-redash/"/>
     <hyperlink ref="F88" r:id="rId3" location="/zh-cn/react-native-redash" display="链接"/>
-    <hyperlink ref="B95" r:id="rId104" display="react-native-snap-carousel" tooltip="https://github.com/meliorence/react-native-snap-carousel"/>
-    <hyperlink ref="E95" r:id="rId105" display="@react-native-oh-tpl/react-native-snap-carousel" tooltip="https://github.com/react-native-oh-library/react-native-snap-carousel/releases"/>
+    <hyperlink ref="B95" r:id="rId105" display="react-native-snap-carousel" tooltip="https://github.com/meliorence/react-native-snap-carousel"/>
+    <hyperlink ref="E95" r:id="rId106" display="@react-native-oh-tpl/react-native-snap-carousel" tooltip="https://github.com/react-native-oh-library/react-native-snap-carousel/releases"/>
     <hyperlink ref="F95" r:id="rId3" location="/zh-cn/react-native-snap-carousel" display="链接"/>
-    <hyperlink ref="B103" r:id="rId106" display="react-native-transitiongroup" tooltip="https://github.com/madsleejensen/react-native-transitiongroup"/>
-    <hyperlink ref="E103" r:id="rId107" display="@react-native-oh-tpl/react-native-transitiongroup" tooltip="https://github.com/react-native-oh-library/react-native-transitiongroup/releases"/>
+    <hyperlink ref="B103" r:id="rId107" display="react-native-transitiongroup" tooltip="https://github.com/madsleejensen/react-native-transitiongroup"/>
+    <hyperlink ref="E103" r:id="rId108" display="@react-native-oh-tpl/react-native-transitiongroup" tooltip="https://github.com/react-native-oh-library/react-native-transitiongroup/releases"/>
     <hyperlink ref="F103" r:id="rId3" location="/zh-cn/react-native-transitiongroup" display="链接"/>
-    <hyperlink ref="B104" r:id="rId108" display="react-native-translucent-modal" tooltip="https://github.com/23mf/react-native-translucent-modal"/>
-    <hyperlink ref="E104" r:id="rId109" display="@react-native-oh-tpl/react-native-translucent-modal" tooltip="https://github.com/react-native-oh-library/react-native-translucent-modal/releases"/>
+    <hyperlink ref="B104" r:id="rId109" display="react-native-translucent-modal" tooltip="https://github.com/23mf/react-native-translucent-modal"/>
+    <hyperlink ref="E104" r:id="rId110" display="@react-native-oh-tpl/react-native-translucent-modal" tooltip="https://github.com/react-native-oh-library/react-native-translucent-modal/releases"/>
     <hyperlink ref="F104" r:id="rId3" location="/zh-cn/react-native-translucent-modal" display="链接"/>
-    <hyperlink ref="B114" r:id="rId110" display="redux" tooltip="https://github.com/reduxjs/redux"/>
+    <hyperlink ref="B114" r:id="rId111" display="redux" tooltip="https://github.com/reduxjs/redux"/>
     <hyperlink ref="F114" r:id="rId3" location="/zh-cn/redux" display="链接"/>
-    <hyperlink ref="B116" r:id="rId111" display="redux-logger" tooltip="https://github.com/LogRocket/redux-logger"/>
+    <hyperlink ref="B116" r:id="rId112" display="redux-logger" tooltip="https://github.com/LogRocket/redux-logger"/>
     <hyperlink ref="F116" r:id="rId3" location="/zh-cn/redux-logger" display="链接"/>
-    <hyperlink ref="B117" r:id="rId112" display="redux-persist" tooltip="https://github.com/rt2zz/redux-persist"/>
+    <hyperlink ref="B117" r:id="rId113" display="redux-persist" tooltip="https://github.com/rt2zz/redux-persist"/>
     <hyperlink ref="F117" r:id="rId3" location="/zh-cn/redux-persist" display="链接"/>
-    <hyperlink ref="B24" r:id="rId113" display="axios" tooltip="https://github.com/axios/axios"/>
+    <hyperlink ref="B24" r:id="rId114" display="axios" tooltip="https://github.com/axios/axios"/>
     <hyperlink ref="F24" r:id="rId3" location="/zh-cn/axios" display="链接"/>
-    <hyperlink ref="B26" r:id="rId114" display="dayJs" tooltip="https://github.com/iamkun/dayjs?tab=readme-ov-file"/>
+    <hyperlink ref="B26" r:id="rId115" display="dayJs" tooltip="https://github.com/iamkun/dayjs?tab=readme-ov-file"/>
     <hyperlink ref="F26" r:id="rId3" location="/zh-cn/dayjs" display="链接"/>
-    <hyperlink ref="B28" r:id="rId115" display="EventBus" tooltip="https://github.com/krasimir/EventBus"/>
+    <hyperlink ref="B28" r:id="rId116" display="EventBus" tooltip="https://github.com/krasimir/EventBus"/>
     <hyperlink ref="F28" r:id="rId3" location="/zh-cn/EventBus" display="链接"/>
-    <hyperlink ref="B30" r:id="rId116" display="immer" tooltip="https://github.com/immerjs/immer"/>
+    <hyperlink ref="B30" r:id="rId117" display="immer" tooltip="https://github.com/immerjs/immer"/>
     <hyperlink ref="F30" r:id="rId3" location="/zh-cn/immer" display="链接"/>
-    <hyperlink ref="B32" r:id="rId117" display="JsBarCode" tooltip="https://github.com/lindell/JsBarcode"/>
+    <hyperlink ref="B32" r:id="rId118" display="JsBarCode" tooltip="https://github.com/lindell/JsBarcode"/>
     <hyperlink ref="F32" r:id="rId3" location="/zh-cn/jsbarcode" display="链接"/>
-    <hyperlink ref="B39" r:id="rId118" display="Moment" tooltip="https://github.com/moment/moment"/>
+    <hyperlink ref="B39" r:id="rId119" display="Moment" tooltip="https://github.com/moment/moment"/>
     <hyperlink ref="F39" r:id="rId3" location="/zh-cn/moment" display="链接"/>
-    <hyperlink ref="B42" r:id="rId119" display="qrcode-generator" tooltip="https://github.com/kazuhikoarase/qrcode-generator"/>
+    <hyperlink ref="B42" r:id="rId120" display="qrcode-generator" tooltip="https://github.com/kazuhikoarase/qrcode-generator"/>
     <hyperlink ref="F42" r:id="rId3" location="/zh-cn/qrcode-generator" display="链接"/>
-    <hyperlink ref="B43" r:id="rId120" display="react-ahooks" tooltip="https://github.com/alibaba/hooks"/>
+    <hyperlink ref="B43" r:id="rId121" display="react-ahooks" tooltip="https://github.com/alibaba/hooks"/>
     <hyperlink ref="F43" r:id="rId3" location="/zh-cn/react-ahooks" display="链接"/>
-    <hyperlink ref="B45" r:id="rId121" display="react-lifecycles-compat" tooltip="https://github.com/reactjs/react-lifecycles-compat"/>
+    <hyperlink ref="B45" r:id="rId122" display="react-lifecycles-compat" tooltip="https://github.com/reactjs/react-lifecycles-compat"/>
     <hyperlink ref="F45" r:id="rId3" location="/zh-cn/react-lifecycles-compat" display="链接"/>
-    <hyperlink ref="B47" r:id="rId122" display="react-native-animate-number" tooltip="https://github.com/wkh237/react-native-animate-number"/>
+    <hyperlink ref="B47" r:id="rId123" display="react-native-animate-number" tooltip="https://github.com/wkh237/react-native-animate-number"/>
     <hyperlink ref="F47" r:id="rId3" location="/zh-cn/react-native-animate-number" display="链接"/>
-    <hyperlink ref="B51" r:id="rId123" display="react-native-blob-util" tooltip="https://github.com/react-native-oh-library/react-native-blob-util"/>
-    <hyperlink ref="E51" r:id="rId124" display="@react-native-oh-tpl/react-native-blob-util" tooltip="https://github.com/react-native-oh-library/react-native-blob-util/releases"/>
+    <hyperlink ref="B51" r:id="rId124" display="react-native-blob-util" tooltip="https://github.com/react-native-oh-library/react-native-blob-util"/>
+    <hyperlink ref="E51" r:id="rId125" display="@react-native-oh-tpl/react-native-blob-util" tooltip="https://github.com/react-native-oh-library/react-native-blob-util/releases"/>
     <hyperlink ref="F51" r:id="rId3" location="/zh-cn/react-native-blob-util" display="链接"/>
-    <hyperlink ref="B52" r:id="rId125" display="react-native-canvas" tooltip="https://github.com/iddan/react-native-canvas"/>
+    <hyperlink ref="B52" r:id="rId126" display="react-native-canvas" tooltip="https://github.com/iddan/react-native-canvas"/>
     <hyperlink ref="F52" r:id="rId3" location="/zh-cn/react-native-canvas" display="链接"/>
-    <hyperlink ref="B54" r:id="rId126" display="react-native-confirmation-code-field" tooltip="https://github.com/retyui/react-native-confirmation-code-field"/>
+    <hyperlink ref="B54" r:id="rId127" display="react-native-confirmation-code-field" tooltip="https://github.com/retyui/react-native-confirmation-code-field"/>
     <hyperlink ref="F54" r:id="rId3" location="/zh-cn/react-native-confirmation-code-field" display="链接"/>
-    <hyperlink ref="B58" r:id="rId127" display="react-native-drawer-layout-polyfill" tooltip="https://github.com/rnc-archive/react-native-drawer-layout-polyfill"/>
+    <hyperlink ref="B58" r:id="rId128" display="react-native-drawer-layout-polyfill" tooltip="https://github.com/rnc-archive/react-native-drawer-layout-polyfill"/>
     <hyperlink ref="F58" r:id="rId3" location="/zh-cn/react-native-drawer-layout-polyfill" display="链接"/>
-    <hyperlink ref="B59" r:id="rId128" display="react-native-echarts-pro" tooltip="https://github.com/supervons/react-native-echarts-pro"/>
+    <hyperlink ref="B59" r:id="rId129" display="react-native-echarts-pro" tooltip="https://github.com/supervons/react-native-echarts-pro"/>
     <hyperlink ref="F59" r:id="rId3" location="/zh-cn/react-native-echarts-pro" display="链接"/>
-    <hyperlink ref="B62" r:id="rId129" display="react-native-fit-Image" tooltip="https://github.com/huiseoul/react-native-fit-image"/>
-    <hyperlink ref="E62" r:id="rId130" display="@react-native-oh-tpl/react-native-fit-Image" tooltip="https://github.com/huiseoul/react-native-fit-image/releases"/>
+    <hyperlink ref="B62" r:id="rId130" display="react-native-fit-Image" tooltip="https://github.com/huiseoul/react-native-fit-image"/>
+    <hyperlink ref="E62" r:id="rId131" display="@react-native-oh-tpl/react-native-fit-Image" tooltip="https://github.com/huiseoul/react-native-fit-image/releases"/>
     <hyperlink ref="F62" r:id="rId3" location="/zh-cn/react-native-fit-Image" display="链接"/>
-    <hyperlink ref="B65" r:id="rId131" display="react-native-image-editor" tooltip="https://github.com/react-native-oh-library/react-native-image-editor"/>
-    <hyperlink ref="E65" r:id="rId132" display="@react-native-oh-tpl/react-native-image-editor" tooltip="https://github.com/react-native-oh-library/react-native-image-editor/releases"/>
+    <hyperlink ref="B65" r:id="rId132" display="react-native-image-editor" tooltip="https://github.com/react-native-oh-library/react-native-image-editor"/>
+    <hyperlink ref="E65" r:id="rId133" display="@react-native-oh-tpl/react-native-image-editor" tooltip="https://github.com/react-native-oh-library/react-native-image-editor/releases"/>
     <hyperlink ref="F65" r:id="rId3" location="/zh-cn/react-native-image-editor" display="链接"/>
-    <hyperlink ref="B67" r:id="rId133" display="react-native-image-viewer" tooltip="https://github.com/react-native-oh-library/react-native-image-viewer"/>
-    <hyperlink ref="E67" r:id="rId134" display="react-native-image-viewer" tooltip="https://github.com/react-native-oh-library/react-native-image-viewer/releases"/>
+    <hyperlink ref="B67" r:id="rId134" display="react-native-image-viewer" tooltip="https://github.com/react-native-oh-library/react-native-image-viewer"/>
+    <hyperlink ref="E67" r:id="rId135" display="react-native-image-viewer" tooltip="https://github.com/react-native-oh-library/react-native-image-viewer/releases"/>
     <hyperlink ref="F67" r:id="rId3" location="/zh-cn/react-native-image-viewer" display="链接"/>
-    <hyperlink ref="B69" r:id="rId135" display="react-native-image-zoom" tooltip="https://github.com/react-native-oh-library/react-native-image-zoom"/>
-    <hyperlink ref="E69" r:id="rId136" display="@react-native-oh-tpl/react-native-image-zoom" tooltip="https://github.com/react-native-oh-library/react-native-image-zoom/releases"/>
+    <hyperlink ref="B69" r:id="rId136" display="react-native-image-zoom" tooltip="https://github.com/react-native-oh-library/react-native-image-zoom"/>
+    <hyperlink ref="E69" r:id="rId137" display="@react-native-oh-tpl/react-native-image-zoom" tooltip="https://github.com/react-native-oh-library/react-native-image-zoom/releases"/>
     <hyperlink ref="F69" r:id="rId3" location="/zh-cn/react-native-image-zoom" display="链接"/>
-    <hyperlink ref="B70" r:id="rId137" display="react-native-intersection-observer" tooltip="https://github.com/react-native-oh-library/react-native-intersection-observer"/>
-    <hyperlink ref="E70" r:id="rId138" display="@react-native-oh-tpl/react-native-intersection-observer" tooltip="https://github.com/react-native-oh-library/react-native-intersection-observer/releases"/>
+    <hyperlink ref="B70" r:id="rId138" display="react-native-intersection-observer" tooltip="https://github.com/react-native-oh-library/react-native-intersection-observer"/>
+    <hyperlink ref="E70" r:id="rId139" display="@react-native-oh-tpl/react-native-intersection-observer" tooltip="https://github.com/react-native-oh-library/react-native-intersection-observer/releases"/>
     <hyperlink ref="F70" r:id="rId3" location="/zh-cn/react-native-intersection-observer" display="链接"/>
-    <hyperlink ref="B68" r:id="rId139" display="react-native-image-viewing" tooltip="https://github.com/react-native-oh-library/react-native-image-viewing"/>
-    <hyperlink ref="E68" r:id="rId140" display="@react-native-oh-tpl/react-native-image-viewing" tooltip="https://github.com/react-native-oh-library/react-native-image-viewing/releases"/>
+    <hyperlink ref="B68" r:id="rId140" display="react-native-image-viewing" tooltip="https://github.com/react-native-oh-library/react-native-image-viewing"/>
+    <hyperlink ref="E68" r:id="rId141" display="@react-native-oh-tpl/react-native-image-viewing" tooltip="https://github.com/react-native-oh-library/react-native-image-viewing/releases"/>
     <hyperlink ref="F68" r:id="rId3" location="/zh-cn/react-native-image-viewing" display="链接"/>
-    <hyperlink ref="B74" r:id="rId141" display="react-native-markdown-display" tooltip="https://github.com/react-native-oh-library/react-native-markdown-display/tree/sig"/>
-    <hyperlink ref="E74" r:id="rId142" display="@react-native-oh-tpl/react-native-markdown-display" tooltip="https://github.com/react-native-oh-library/react-native-markdown-display/releases"/>
+    <hyperlink ref="B74" r:id="rId142" display="react-native-markdown-display" tooltip="https://github.com/react-native-oh-library/react-native-markdown-display/tree/sig"/>
+    <hyperlink ref="E74" r:id="rId143" display="@react-native-oh-tpl/react-native-markdown-display" tooltip="https://github.com/react-native-oh-library/react-native-markdown-display/releases"/>
     <hyperlink ref="F74" r:id="rId3" location="/zh-cn/react-native-markdown-display" display="链接"/>
-    <hyperlink ref="B75" r:id="rId143" display="react-native-marquee" tooltip="https://github.com/react-native-oh-library/react-native-marquee"/>
-    <hyperlink ref="E75" r:id="rId144" display="@react-native-oh-tpl/react-native-marquee" tooltip="https://github.com/react-native-oh-library/react-native-marquee/releases"/>
+    <hyperlink ref="B75" r:id="rId144" display="react-native-marquee" tooltip="https://github.com/react-native-oh-library/react-native-marquee"/>
+    <hyperlink ref="E75" r:id="rId145" display="@react-native-oh-tpl/react-native-marquee" tooltip="https://github.com/react-native-oh-library/react-native-marquee/releases"/>
     <hyperlink ref="F75" r:id="rId3" location="/zh-cn/react-native-marquee" display="链接"/>
-    <hyperlink ref="B80" r:id="rId145" display="react-native-popover-view" tooltip="https://github.com/react-native-oh-library/react-native-popover-view"/>
-    <hyperlink ref="E80" r:id="rId146" display="@react-native-oh-tpl/react-native-popover-view" tooltip="https://github.com/react-native-oh-library/react-native-popover-view/releases"/>
+    <hyperlink ref="B80" r:id="rId146" display="react-native-popover-view" tooltip="https://github.com/react-native-oh-library/react-native-popover-view"/>
+    <hyperlink ref="E80" r:id="rId147" display="@react-native-oh-tpl/react-native-popover-view" tooltip="https://github.com/react-native-oh-library/react-native-popover-view/releases"/>
     <hyperlink ref="F80" r:id="rId3" location="/zh-cn/react-native-popover-view" display="链接"/>
-    <hyperlink ref="B81" r:id="rId147" display="react-native-popup-menu" tooltip="https://github.com/instea/react-native-popup-menu"/>
+    <hyperlink ref="B81" r:id="rId148" display="react-native-popup-menu" tooltip="https://github.com/instea/react-native-popup-menu"/>
     <hyperlink ref="F81" r:id="rId3" location="/zh-cn/react-native-popup-menu" display="链接"/>
-    <hyperlink ref="B83" r:id="rId148" display="react-native-pull" tooltip="https://github.com/react-native-oh-library/react-native-pull"/>
-    <hyperlink ref="E83" r:id="rId149" display="@react-native-oh-tpl/react-native-pull" tooltip="https://github.com/react-native-oh-library/react-native-pull/releases"/>
+    <hyperlink ref="B83" r:id="rId149" display="react-native-pull" tooltip="https://github.com/react-native-oh-library/react-native-pull"/>
+    <hyperlink ref="E83" r:id="rId150" display="@react-native-oh-tpl/react-native-pull" tooltip="https://github.com/react-native-oh-library/react-native-pull/releases"/>
     <hyperlink ref="F83" r:id="rId3" location="/zh-cn/react-native-pull" display="链接"/>
-    <hyperlink ref="B87" r:id="rId150" display="react-native-reanimated-table" tooltip="https://github.com/dohooo/react-native-reanimated-table"/>
+    <hyperlink ref="B87" r:id="rId151" display="react-native-reanimated-table" tooltip="https://github.com/dohooo/react-native-reanimated-table"/>
     <hyperlink ref="F87" r:id="rId3" location="/zh-cn/react-native-reanimated-table" display="链接"/>
-    <hyperlink ref="B92" r:id="rId151" display="react-native-scrollable-tab-view" tooltip="https://github.com/react-native-oh-library/react-native-scrollable-tab-view"/>
+    <hyperlink ref="B92" r:id="rId152" display="react-native-scrollable-tab-view" tooltip="https://github.com/react-native-oh-library/react-native-scrollable-tab-view"/>
     <hyperlink ref="F92" r:id="rId3" location="/zh-cn/react-native-scrollable-tab-view" display="链接"/>
-    <hyperlink ref="B97" r:id="rId152" display="react-native-stickyheader" tooltip="https://github.com/react-native-oh-library/react-native-stickyheader"/>
-    <hyperlink ref="E97" r:id="rId153" display="@react-native-oh-tpl/react-native-stickyheader" tooltip="https://github.com/react-native-oh-library/react-native-stickyheader/releases"/>
+    <hyperlink ref="B97" r:id="rId153" display="react-native-stickyheader" tooltip="https://github.com/react-native-oh-library/react-native-stickyheader"/>
+    <hyperlink ref="E97" r:id="rId154" display="@react-native-oh-tpl/react-native-stickyheader" tooltip="https://github.com/react-native-oh-library/react-native-stickyheader/releases"/>
     <hyperlink ref="F97" r:id="rId3" location="/zh-cn/react-native-stickyheader" display="链接"/>
-    <hyperlink ref="B99" r:id="rId127" display="react-native-swipe-list-view" tooltip="https://github.com/rnc-archive/react-native-drawer-layout-polyfill"/>
+    <hyperlink ref="B99" r:id="rId128" display="react-native-swipe-list-view" tooltip="https://github.com/rnc-archive/react-native-drawer-layout-polyfill"/>
     <hyperlink ref="F99" r:id="rId3" location="/zh-cn/react-native-swipe-list-view" display="链接"/>
-    <hyperlink ref="B100" r:id="rId154" display="react-native-swiper" tooltip="https://github.com/leecade/react-native-swiper"/>
+    <hyperlink ref="B100" r:id="rId155" display="react-native-swiper" tooltip="https://github.com/leecade/react-native-swiper"/>
     <hyperlink ref="F100" r:id="rId3" location="/zh-cn/react-native-swiper" display="链接"/>
-    <hyperlink ref="B109" r:id="rId155" display="react-native-worklets-core" tooltip="https://github.com/react-native-oh-library/react-native-worklets-core"/>
-    <hyperlink ref="E109" r:id="rId156" display="@react-native-oh-tpl/react-native-worklets-core" tooltip="https://github.com/react-native-oh-library/react-native-worklets-core/releases"/>
+    <hyperlink ref="B109" r:id="rId156" display="react-native-worklets-core" tooltip="https://github.com/react-native-oh-library/react-native-worklets-core"/>
+    <hyperlink ref="E109" r:id="rId157" display="@react-native-oh-tpl/react-native-worklets-core" tooltip="https://github.com/react-native-oh-library/react-native-worklets-core/releases"/>
     <hyperlink ref="F109" r:id="rId3" location="/zh-cn/react-native-worklets-core" display="链接"/>
-    <hyperlink ref="B112" r:id="rId157" display="react-use" tooltip="https://github.com/zenghongtu/react-use"/>
+    <hyperlink ref="B112" r:id="rId158" display="react-use" tooltip="https://github.com/zenghongtu/react-use"/>
     <hyperlink ref="F112" r:id="rId3" location="/zh-cn/react-use" display="链接"/>
-    <hyperlink ref="B119" r:id="rId158" display="redux-toolkit" tooltip="https://github.com/reduxjs/redux-toolkit"/>
-    <hyperlink ref="F119" r:id="rId159" display="链接"/>
-    <hyperlink ref="B102" r:id="rId160" display="react-native-text-size" tooltip="https://github.com/aMarCruz/react-native-text-size"/>
-    <hyperlink ref="E102" r:id="rId161" display="@react-native-oh-tpl/react-native-text-size" tooltip="https://github.com/react-native-oh-library/react-native-text-size/releases"/>
+    <hyperlink ref="B119" r:id="rId159" display="redux-toolkit" tooltip="https://github.com/reduxjs/redux-toolkit"/>
+    <hyperlink ref="F119" r:id="rId160" display="链接"/>
+    <hyperlink ref="B102" r:id="rId161" display="react-native-text-size" tooltip="https://github.com/aMarCruz/react-native-text-size"/>
+    <hyperlink ref="E102" r:id="rId162" display="@react-native-oh-tpl/react-native-text-size" tooltip="https://github.com/react-native-oh-library/react-native-text-size/releases"/>
     <hyperlink ref="F102" r:id="rId3" location="/zh-cn/react-native-text-size" display="链接"/>
-    <hyperlink ref="B111" r:id="rId162" display="react-router-dom" tooltip="https://github.com/remix-run/react-router"/>
+    <hyperlink ref="B111" r:id="rId163" display="react-router-dom" tooltip="https://github.com/remix-run/react-router"/>
     <hyperlink ref="F111" r:id="rId3" location="/zh-cn/react-router-dom" display="链接"/>
-    <hyperlink ref="B115" r:id="rId163" display="redux-actions" tooltip="https://github.com/redux-utilities/redux-actions"/>
+    <hyperlink ref="B115" r:id="rId164" display="redux-actions" tooltip="https://github.com/redux-utilities/redux-actions"/>
     <hyperlink ref="F115" r:id="rId3" location="/zh-cn/redux-actions" display="链接"/>
-    <hyperlink ref="B118" r:id="rId164" display="redux-thunk" tooltip="https://github.com/reduxjs/redux-thunk"/>
+    <hyperlink ref="B118" r:id="rId165" display="redux-thunk" tooltip="https://github.com/reduxjs/redux-thunk"/>
     <hyperlink ref="F118" r:id="rId3" location="/zh-cn/redux-thunk" display="链接"/>
-    <hyperlink ref="B48" r:id="rId165" display="react-native-aria" tooltip="https://github.com/gluestack/react-native-aria/"/>
+    <hyperlink ref="B48" r:id="rId166" display="react-native-aria" tooltip="https://github.com/gluestack/react-native-aria/"/>
     <hyperlink ref="F48" r:id="rId3" location="/zh-cn/react-native-aria" display="链接"/>
-    <hyperlink ref="B82" r:id="rId166" display="react-native-progress" tooltip="https://github.com/oblador/react-native-progress"/>
-    <hyperlink ref="E82" r:id="rId167" display="@react-native-oh-tpl/react-native-progress" tooltip="https://github.com/react-native-oh-library/react-native-progress/releases"/>
+    <hyperlink ref="B82" r:id="rId167" display="react-native-progress" tooltip="https://github.com/oblador/react-native-progress"/>
+    <hyperlink ref="E82" r:id="rId168" display="@react-native-oh-tpl/react-native-progress" tooltip="https://github.com/react-native-oh-library/react-native-progress/releases"/>
     <hyperlink ref="F82" r:id="rId3" location="/zh-cn/react-native-progress" display="链接"/>
-    <hyperlink ref="B63" r:id="rId168" display="react-native-fs" tooltip="https://github.com/itinance/react-native-fs"/>
-    <hyperlink ref="E63" r:id="rId169" display="@react-native-oh-tpl/react-native-fs" tooltip="https://github.com/react-native-oh-library/react-native-fs/releases"/>
+    <hyperlink ref="B63" r:id="rId169" display="react-native-fs" tooltip="https://github.com/itinance/react-native-fs"/>
+    <hyperlink ref="E63" r:id="rId170" display="@react-native-oh-tpl/react-native-fs" tooltip="https://github.com/react-native-oh-library/react-native-fs/releases"/>
     <hyperlink ref="F63" r:id="rId3" location="/zh-cn/react-native-fs" display="链接"/>
-    <hyperlink ref="B71" r:id="rId170" display="react-native-keyboard-aware-scroll-view" tooltip="https://github.com/APSL/react-native-keyboard-aware-scroll-view"/>
-    <hyperlink ref="E71" r:id="rId171" display="@react-native-oh-tpl/react-native-keyboard-aware-scroll-view" tooltip="https://github.com/react-native-oh-library/react-native-keyboard-aware-scroll-view/releases"/>
+    <hyperlink ref="B71" r:id="rId171" display="react-native-keyboard-aware-scroll-view" tooltip="https://github.com/APSL/react-native-keyboard-aware-scroll-view"/>
+    <hyperlink ref="E71" r:id="rId172" display="@react-native-oh-tpl/react-native-keyboard-aware-scroll-view" tooltip="https://github.com/react-native-oh-library/react-native-keyboard-aware-scroll-view/releases"/>
     <hyperlink ref="F71" r:id="rId3" location="/zh-cn/react-native-keyboard-aware-scroll-view" display="链接"/>
-    <hyperlink ref="B79" r:id="rId172" display="react-native-permissions" tooltip="https://github.com/zoontek/react-native-permissions"/>
-    <hyperlink ref="E79" r:id="rId173" display="@react-native-oh-tpl/react-native-permissions" tooltip="https://github.com/react-native-oh-library/react-native-permissions/releases"/>
+    <hyperlink ref="B79" r:id="rId173" display="react-native-permissions" tooltip="https://github.com/zoontek/react-native-permissions"/>
+    <hyperlink ref="E79" r:id="rId174" display="@react-native-oh-tpl/react-native-permissions" tooltip="https://github.com/react-native-oh-library/react-native-permissions/releases"/>
     <hyperlink ref="F79" r:id="rId3" location="/zh-cn/react-native-permissions" display="链接"/>
-    <hyperlink ref="B57" r:id="rId174" display="react-native-drag-sort" tooltip="https://github.com/mochixuan/react-native-drag-sort"/>
+    <hyperlink ref="B57" r:id="rId175" display="react-native-drag-sort" tooltip="https://github.com/mochixuan/react-native-drag-sort"/>
     <hyperlink ref="F57" r:id="rId3" location="/zh-cn/react-native-drag-sort" display="链接"/>
-    <hyperlink ref="B96" r:id="rId175" display="react-native-sound" tooltip="https://github.com/zmxv/react-native-sound"/>
-    <hyperlink ref="E96" r:id="rId176" display="@react-native-oh-tpl/react-native-sound" tooltip="https://github.com/react-native-oh-library/react-native-sound/releases"/>
+    <hyperlink ref="B96" r:id="rId176" display="react-native-sound" tooltip="https://github.com/zmxv/react-native-sound"/>
+    <hyperlink ref="E96" r:id="rId177" display="@react-native-oh-tpl/react-native-sound" tooltip="https://github.com/react-native-oh-library/react-native-sound/releases"/>
     <hyperlink ref="F96" r:id="rId3" location="/zh-cn/react-native-sound" display="链接"/>
-    <hyperlink ref="B86" r:id="rId177" display="react-native-reanimated-carousel" tooltip="https://github.com/dohooo/react-native-reanimated-carousel"/>
+    <hyperlink ref="B86" r:id="rId178" display="react-native-reanimated-carousel" tooltip="https://github.com/dohooo/react-native-reanimated-carousel"/>
     <hyperlink ref="F86" r:id="rId3" location="/zh-cn/react-native-reanimated-carousel" display="链接"/>
-    <hyperlink ref="B14" r:id="rId178" display="@react-native-community/toolbar-android" tooltip="https://github.com/react-native-toolbar-android/toolbar-android"/>
-    <hyperlink ref="E14" r:id="rId179" display="@react-native-oh-tpl/toolbar-android" tooltip="https://github.com/react-native-oh-library/toolbar-android/releases"/>
+    <hyperlink ref="B14" r:id="rId179" display="@react-native-community/toolbar-android" tooltip="https://github.com/react-native-toolbar-android/toolbar-android"/>
+    <hyperlink ref="E14" r:id="rId180" display="@react-native-oh-tpl/toolbar-android" tooltip="https://github.com/react-native-oh-library/toolbar-android/releases"/>
     <hyperlink ref="F14" r:id="rId3" location="/zh-cn/react-native-toolbar-android" display="链接"/>
-    <hyperlink ref="B110" r:id="rId180" display="react-redux" tooltip="https://github.com/reduxjs/react-redux"/>
+    <hyperlink ref="B110" r:id="rId181" display="react-redux" tooltip="https://github.com/reduxjs/react-redux"/>
     <hyperlink ref="F110" r:id="rId3" location="/zh-cn/react-redux" display="链接"/>
-    <hyperlink ref="B76" r:id="rId181" display="react-native-MJRefresh" tooltip="https://github.com/react-native-studio/react-native-MJRefresh"/>
-    <hyperlink ref="E76" r:id="rId182" display="@react-native-oh-tpl/react-native-mjrefresh" tooltip="https://github.com/react-native-oh-library/react-native-MJRefresh/releases"/>
-    <hyperlink ref="E92" r:id="rId183" display="@react-native-oh-tpl/react-native-scrollable-tab-view" tooltip="https://github.com/react-native-oh-library/react-native-scrollable-tab-view/releases"/>
+    <hyperlink ref="B76" r:id="rId182" display="react-native-MJRefresh" tooltip="https://github.com/react-native-studio/react-native-MJRefresh"/>
+    <hyperlink ref="E76" r:id="rId183" display="@react-native-oh-tpl/react-native-mjrefresh" tooltip="https://github.com/react-native-oh-library/react-native-MJRefresh/releases"/>
+    <hyperlink ref="E92" r:id="rId184" display="@react-native-oh-tpl/react-native-scrollable-tab-view" tooltip="https://github.com/react-native-oh-library/react-native-scrollable-tab-view/releases"/>
     <hyperlink ref="F55" r:id="rId3" location="/zh-cn/react-native-crypto-js" display="链接"/>
     <hyperlink ref="F76" r:id="rId3" location="/zh-cn/react-native-MJRefresh" display="链接"/>
-    <hyperlink ref="F123" r:id="rId184" display="链接"/>
-    <hyperlink ref="F124" r:id="rId185" display="链接"/>
-    <hyperlink ref="E124" r:id="rId186" display="@react-native-oh-tpl/react-native-sortable-list"/>
-    <hyperlink ref="B124" r:id="rId187" display="react-native-sortable-list"/>
-    <hyperlink ref="B123" r:id="rId188" display="react-native-sensors"/>
-    <hyperlink ref="E123" r:id="rId189" display="@react-native-oh-tpl/react-native-sensors"/>
-    <hyperlink ref="B126" r:id="rId190" display="react-native-image-sequence-2"/>
-    <hyperlink ref="E126" r:id="rId191" display="@react-native-oh-tpl/react-native-image-sequence-2"/>
+    <hyperlink ref="F123" r:id="rId185" display="链接"/>
+    <hyperlink ref="F124" r:id="rId186" display="链接"/>
+    <hyperlink ref="E124" r:id="rId187" display="@react-native-oh-tpl/react-native-sortable-list"/>
+    <hyperlink ref="B124" r:id="rId188" display="react-native-sortable-list"/>
+    <hyperlink ref="B123" r:id="rId189" display="react-native-sensors"/>
+    <hyperlink ref="E123" r:id="rId190" display="@react-native-oh-tpl/react-native-sensors"/>
+    <hyperlink ref="B126" r:id="rId191" display="react-native-image-sequence-2"/>
+    <hyperlink ref="E126" r:id="rId192" display="@react-native-oh-tpl/react-native-image-sequence-2"/>
     <hyperlink ref="F126" r:id="rId3" location="/zh-cn/react-native-sequence-2" display="链接"/>
-    <hyperlink ref="B127" r:id="rId192" display="react-native-feather"/>
+    <hyperlink ref="B127" r:id="rId193" display="react-native-feather"/>
     <hyperlink ref="F127" r:id="rId3" location="/zh-cn/react-native-feather" display="链接"/>
-    <hyperlink ref="B125" r:id="rId193" display="react-native-easy-toast"/>
+    <hyperlink ref="B125" r:id="rId194" display="react-native-easy-toast"/>
     <hyperlink ref="F125" r:id="rId3" location="/zh-cn/react-native-sequence-2" display="链接"/>
-    <hyperlink ref="B128" r:id="rId194" display="@react-navigation/native-stack"/>
-    <hyperlink ref="E128" r:id="rId195" display="@react-native-oh-tpl/native-stack"/>
+    <hyperlink ref="B128" r:id="rId195" display="@react-navigation/native-stack"/>
+    <hyperlink ref="E128" r:id="rId196" display="@react-native-oh-tpl/native-stack"/>
     <hyperlink ref="F128" r:id="rId3" location="/zh-cn/react-navigation-native-stack.md" display="链接"/>
+    <hyperlink ref="B129" r:id="rId197" display="react-native-waterfall-flow"/>
+    <hyperlink ref="F129" r:id="rId198" display="链接"/>
+    <hyperlink ref="B130" r:id="rId199" display="react-native-vconsole"/>
+    <hyperlink ref="F130" r:id="rId200" display="链接"/>
+    <hyperlink ref="B131" r:id="rId201" display="better-banner"/>
+    <hyperlink ref="F131" r:id="rId202" display="链接"/>
+    <hyperlink ref="B132" r:id="rId203" display="react-native-ezswiper"/>
+    <hyperlink ref="F132" r:id="rId204" display="链接"/>
+    <hyperlink ref="B133" r:id="rId205" display="react-native-image-header-scroll-view"/>
+    <hyperlink ref="F133" r:id="rId206" display="链接"/>
+    <hyperlink ref="B134" r:id="rId207" display="react-native-linear-gradient-text"/>
+    <hyperlink ref="F134" r:id="rId208" display="链接"/>
+    <hyperlink ref="B135" r:id="rId209" display="react-native-marquee-ab"/>
+    <hyperlink ref="F135" r:id="rId210" display="链接"/>
+    <hyperlink ref="B136" r:id="rId211" display="react-native-reconnecting-websocket"/>
+    <hyperlink ref="F136" r:id="rId212" display="链接"/>
+    <hyperlink ref="B137" r:id="rId213" display="react-native-json-tree"/>
+    <hyperlink ref="F137" r:id="rId214" display="链接"/>
+    <hyperlink ref="B138" r:id="rId215" display="react-native-image-gallery"/>
+    <hyperlink ref="F138" r:id="rId216" display="链接"/>
+    <hyperlink ref="E138" r:id="rId217" display="@react-native-oh-tpl/react-native-image-gallery"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
docs: [Issues: #I9V1TD] 修改Menu跳转链接
</commit_message>
<xml_diff>
--- a/Menu.xlsx
+++ b/Menu.xlsx
@@ -2262,8 +2262,8 @@
   <sheetPr/>
   <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="I111" sqref="I111"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -2296,7 +2296,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" ht="14.25" spans="1:6">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -4770,7 +4770,7 @@
       <c r="E125" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F125" s="8" t="s">
+      <c r="F125" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4790,7 +4790,7 @@
       <c r="E126" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="F126" s="8" t="s">
+      <c r="F126" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4830,7 +4830,7 @@
       <c r="E128" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="F128" s="8" t="s">
+      <c r="F128" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4850,7 +4850,7 @@
       <c r="E129" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="F129" s="8" t="s">
+      <c r="F129" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -5044,344 +5044,344 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="@react-native-async-storage/async-storage" tooltip="https://github.com/react-native-async-storage/async-storage"/>
     <hyperlink ref="E2" r:id="rId2" display="@react-native-oh-tpl/async-storage" tooltip="https://github.com/react-native-oh-library/async-storage/releases"/>
-    <hyperlink ref="F2" r:id="rId3" location="/zh-cn/react-native-async-storage-async-storage" display="链接"/>
+    <hyperlink ref="F2" r:id="rId3" display="链接"/>
     <hyperlink ref="B4" r:id="rId4" display="@react-native-clipboard/clipboard" tooltip="https://github.com/react-native-clipboard/clipboard"/>
     <hyperlink ref="E4" r:id="rId5" display="@react-native-oh-tpl/clipboard" tooltip="https://github.com/react-native-oh-library/clipboard/releases"/>
-    <hyperlink ref="F4" r:id="rId3" location="/zh-cn/react-native-clipboard-clipboard" display="链接"/>
-    <hyperlink ref="B7" r:id="rId6" display="@react-native-community/datetimepicker" tooltip="https://github.com/react-native-datetimepicker/datetimepicker"/>
-    <hyperlink ref="E7" r:id="rId7" display="@react-native-oh-tpl/datetimepicker" tooltip="https://github.com/react-native-oh-library/datetimepicker/releases"/>
-    <hyperlink ref="F7" r:id="rId3" location="/zh-cn/react-native-community-datetimepicker" display="链接"/>
-    <hyperlink ref="B23" r:id="rId8" display="@shopify/flash-list" tooltip="https://github.com/Shopify/flash-list"/>
-    <hyperlink ref="E23" r:id="rId9" display="@react-native-oh-tpl/flash-list" tooltip="https://github.com/react-native-oh-library/flash-list/releases"/>
-    <hyperlink ref="F23" r:id="rId3" location="/zh-cn/shopify-flash-list" display="链接"/>
-    <hyperlink ref="B36" r:id="rId10" display="lottie-react-native" tooltip="https://github.com/lottie-react-native/lottie-react-native"/>
-    <hyperlink ref="E36" r:id="rId11" display="@react-native-oh-tpl/lottie-react-native" tooltip="https://github.com/react-native-oh-library/lottie-react-native/releases"/>
-    <hyperlink ref="F36" r:id="rId3" location="/zh-cn/lottie-react-native" display="链接"/>
-    <hyperlink ref="B17" r:id="rId12" display="@react-native-picker/picker" tooltip="https://github.com/react-native-picker/picker"/>
-    <hyperlink ref="E17" r:id="rId13" display="@react-native-oh-tpl/picker" tooltip="https://github.com/react-native-oh-library/picker/releases"/>
-    <hyperlink ref="F17" r:id="rId3" location="/zh-cn/react-native-picker-picker" display="链接"/>
-    <hyperlink ref="B10" r:id="rId14" display="@react-native-community/progress-bar-android" tooltip="https://github.com/react-native-progress-view/progress-bar-android"/>
-    <hyperlink ref="E10" r:id="rId15" display="@react-native-oh-tpl/progress-bar-android" tooltip="https://github.com/react-native-oh-library/progress-bar-android/releases"/>
-    <hyperlink ref="F10" r:id="rId3" location="/zh-cn/react-native-community-progress-bar-android" display="链接"/>
-    <hyperlink ref="B6" r:id="rId16" display="@react-native-community/checkbox" tooltip="https://github.com/react-native-checkbox/react-native-checkbox"/>
-    <hyperlink ref="E6" r:id="rId17" display="@react-native-oh-tpl/react-native-checkbox" tooltip="https://github.com/react-native-oh-library/react-native-checkbox/releases"/>
-    <hyperlink ref="F6" r:id="rId3" location="/zh-cn/react-native-community-checkbox" display="链接"/>
-    <hyperlink ref="B60" r:id="rId18" display="react-native-exception-handler" tooltip="https://github.com/a7ul/react-native-exception-handler"/>
-    <hyperlink ref="E60" r:id="rId19" display="@react-native-oh-tpl/react-native-exception-handler" tooltip="https://github.com/react-native-oh-library/react-native-exception-handler/releases"/>
-    <hyperlink ref="F60" r:id="rId3" location="/zh-cn/react-native-exception-handler" display="链接"/>
-    <hyperlink ref="B61" r:id="rId20" display="react-native-fast-image" tooltip="https://github.com/DylanVann/react-native-fast-image"/>
-    <hyperlink ref="E61" r:id="rId21" display="@react-native-oh-tpl/react-native-fast-image" tooltip="https://github.com/react-native-oh-library/react-native-fast-image/releases"/>
-    <hyperlink ref="F61" r:id="rId3" location="/zh-cn/react-native-fast-image" display="链接"/>
-    <hyperlink ref="B64" r:id="rId22" display="react-native-gesture-handler" tooltip="https://github.com/software-mansion/react-native-gesture-handler"/>
-    <hyperlink ref="E64" r:id="rId23" display="@react-native-oh-tpl/react-native-gesture-handler" tooltip="https://github.com/react-native-oh-library/react-native-gesture-handler/releases"/>
-    <hyperlink ref="F64" r:id="rId3" location="/zh-cn/react-native-gesture-handler" display="链接"/>
-    <hyperlink ref="B66" r:id="rId24" display="react-native-image-picker" tooltip="https://github.com/react-native-image-picker/react-native-image-picker"/>
-    <hyperlink ref="E66" r:id="rId25" display="@react-native-oh-tpl/react-native-image-picker" tooltip="https://github.com/react-native-oh-library/react-native-image-picker/releases"/>
-    <hyperlink ref="F66" r:id="rId3" location="/zh-cn/react-native-image-picker" display="链接"/>
-    <hyperlink ref="B72" r:id="rId26" display="react-native-linear-gradient" tooltip="https://github.com/react-native-linear-gradient/react-native-linear-gradient"/>
-    <hyperlink ref="E72" r:id="rId27" display="@react-native-oh-tpl/react-native-linear-gradient" tooltip="https://github.com/react-native-oh-library/react-native-linear-gradient/releases"/>
-    <hyperlink ref="F72" r:id="rId3" location="/zh-cn/react-native-linear-gradient" display="链接"/>
-    <hyperlink ref="B16" r:id="rId28" display="@react-native-masked-view/masked-view" tooltip="https://github.com/react-native-masked-view/masked-view"/>
-    <hyperlink ref="E16" r:id="rId29" display="@react-native-oh-tpl/masked-view" tooltip="https://github.com/react-native-oh-library/masked-view/releases"/>
-    <hyperlink ref="F16" r:id="rId3" location="/zh-cn/react-native-masked-view-masked-view" display="链接"/>
-    <hyperlink ref="B9" r:id="rId30" display="@react-native-community/netinfo" tooltip="https://github.com/react-native-netinfo/react-native-netinfo"/>
-    <hyperlink ref="E9" r:id="rId31" display="@react-native-oh-tpl/netinfo" tooltip="https://github.com/react-native-oh-library/react-native-netinfo/releases"/>
-    <hyperlink ref="F9" r:id="rId3" location="/zh-cn/react-native-community-netinfo" display="链接"/>
-    <hyperlink ref="B77" r:id="rId32" display="react-native-pager-view" tooltip="https://github.com/callstack/react-native-pager-view"/>
-    <hyperlink ref="E77" r:id="rId33" display="@react-native-oh-tpl/react-native-pager-view" tooltip="https://github.com/react-native-oh-library/react-native-pager-view/releases"/>
-    <hyperlink ref="F77" r:id="rId3" location="/zh-cn/react-native-pager-view" display="链接"/>
-    <hyperlink ref="B90" r:id="rId34" display="react-native-safe-area-context" tooltip="https://github.com/th3rdwave/react-native-safe-area-context"/>
-    <hyperlink ref="E90" r:id="rId35" display="@react-native-oh-tpl/react-native-safe-area-context" tooltip="https://github.com/react-native-oh-library/react-native-safe-area-context/releases"/>
-    <hyperlink ref="F90" r:id="rId3" location="/zh-cn/react-native-safe-area-context" display="链接"/>
-    <hyperlink ref="B91" r:id="rId36" display="react-native-screens" tooltip="https://github.com/software-mansion/react-native-screens"/>
-    <hyperlink ref="F91" r:id="rId3" location="/zh-cn/react-native-screens" display="链接"/>
-    <hyperlink ref="B13" r:id="rId37" display="@react-native-community/slider" tooltip="https://github.com/callstack/react-native-slider"/>
-    <hyperlink ref="E13" r:id="rId38" display="@react-native-oh-tpl/slider" tooltip="https://github.com/react-native-oh-library/react-native-slider/releases"/>
-    <hyperlink ref="F13" r:id="rId3" location="/zh-cn/react-native-community-slider" display="链接"/>
-    <hyperlink ref="B94" r:id="rId39" display="react-native-SmartRefreshLayout" tooltip="https://github.com/react-native-studio/react-native-SmartRefreshLayout"/>
-    <hyperlink ref="E94" r:id="rId40" display="@react-native-oh-tpl/react-native-SmartRefreshLayout" tooltip="https://github.com/react-native-oh-library/react-native-SmartRefreshLayout/releases"/>
-    <hyperlink ref="F94" r:id="rId3" location="/zh-cn/react-native-SmartRefreshLayout" display="链接"/>
-    <hyperlink ref="B98" r:id="rId41" display="react-native-svg" tooltip="https://github.com/software-mansion/react-native-svg"/>
-    <hyperlink ref="E98" r:id="rId42" display="@react-native-oh-tpl/react-native-svg" tooltip="https://github.com/react-native-oh-library/react-native-svg/releases"/>
-    <hyperlink ref="F98" r:id="rId3" location="/zh-cn/react-native-svg" display="链接"/>
-    <hyperlink ref="B101" r:id="rId43" display="react-native-tab-view" tooltip="https://github.com/react-navigation/react-navigation/tree/6.x/packages/react-native-tab-view"/>
-    <hyperlink ref="E101" r:id="rId44" display="@react-native-oh-tpl/react-native-tab-view" tooltip="https://github.com/react-native-oh-library/react-navigation/releases"/>
-    <hyperlink ref="F101" r:id="rId3" location="/zh-cn/react-native-tab-view" display="链接"/>
-    <hyperlink ref="B106" r:id="rId45" display="react-native-video" tooltip="https://github.com/react-native-video/react-native-video"/>
-    <hyperlink ref="E106" r:id="rId46" display="@react-native-oh-tpl/react-native-video" tooltip="https://github.com/react-native-oh-library/react-native-video"/>
-    <hyperlink ref="F106" r:id="rId3" location="/zh-cn/react-native-video" display="链接"/>
-    <hyperlink ref="B108" r:id="rId47" display="react-native-webview" tooltip="https://github.com/react-native-webview/react-native-webview"/>
-    <hyperlink ref="E108" r:id="rId48" display="@react-native-oh-tpl/react-native-webview" tooltip="https://github.com/react-native-oh-library/react-native-webview/releases"/>
-    <hyperlink ref="F108" r:id="rId3" location="/zh-cn/react-native-webview" display="链接"/>
-    <hyperlink ref="B20" r:id="rId49" display="@react-navigation/elements" tooltip="https://github.com/react-navigation/react-navigation/tree/6.x/packages/elements"/>
-    <hyperlink ref="E20" r:id="rId44" display="@react-native-oh-tpl/elements" tooltip="https://github.com/react-native-oh-library/react-navigation/releases"/>
-    <hyperlink ref="F20" r:id="rId3" location="/zh-cn/react-navigation-elements" display="链接"/>
-    <hyperlink ref="B25" r:id="rId50" display="crypto-js" tooltip="https://github.com/brix/crypto-js/tree/4.2.0"/>
-    <hyperlink ref="F25" r:id="rId3" location="/zh-cn/crypto-js" display="链接"/>
-    <hyperlink ref="B27" r:id="rId51" display="deepmerge" tooltip="https://github.com/TehShrike/deepmerge"/>
-    <hyperlink ref="F27" r:id="rId3" location="/zh-cn/deepmerge" display="链接"/>
-    <hyperlink ref="B29" r:id="rId52" display="htmlparser2" tooltip="https://github.com/fb55/htmlparser2"/>
-    <hyperlink ref="F29" r:id="rId3" location="/zh-cn/htmlparser2" display="链接"/>
-    <hyperlink ref="B33" r:id="rId53" display="js-beautify" tooltip="https://github.com/beautifier/js-beautify"/>
-    <hyperlink ref="F33" r:id="rId3" location="/zh-cn/js-beautify" display="链接"/>
-    <hyperlink ref="B35" r:id="rId54" display="lodash" tooltip="https://github.com/lodash/lodash/tree/4.17.21"/>
-    <hyperlink ref="F35" r:id="rId3" location="/zh-cn/lodash" display="链接"/>
-    <hyperlink ref="B38" r:id="rId55" display="mobx-react" tooltip="https://github.com/mobxjs/mobx/tree/mobx-react@7.6.0"/>
-    <hyperlink ref="F38" r:id="rId3" location="/zh-cn/mobx-react" display="链接"/>
-    <hyperlink ref="B37" r:id="rId56" display="mobx" tooltip="https://github.com/mobxjs/mobx/tree/mobx@6.10.0"/>
-    <hyperlink ref="F37" r:id="rId3" location="/zh-cn/mobx" display="链接"/>
-    <hyperlink ref="B40" r:id="rId57" display="parse5" tooltip="https://github.com/inikulin/parse5"/>
-    <hyperlink ref="F40" r:id="rId3" location="/zh-cn/parse5" display="链接"/>
-    <hyperlink ref="B41" r:id="rId58" display="prop-types" tooltip="https://github.com/facebook/prop-types/tree/v15.8.1"/>
-    <hyperlink ref="F41" r:id="rId3" location="/zh-cn/prop-types" display="链接"/>
-    <hyperlink ref="B44" r:id="rId59" display="react-i18next" tooltip="https://github.com/i18next/react-i18next"/>
-    <hyperlink ref="F44" r:id="rId3" location="/zh-cn/react-i18next" display="链接"/>
-    <hyperlink ref="B46" r:id="rId60" display="react-native-action-button" tooltip="https://github.com/mastermoo/react-native-action-button"/>
-    <hyperlink ref="F46" r:id="rId3" location="/zh-cn/react-native-action-button" display="链接"/>
-    <hyperlink ref="B49" r:id="rId61" display="react-native-autoheight-webview" tooltip="https://github.com/react-native-oh-library/react-native-autoheight-webview"/>
-    <hyperlink ref="E49" r:id="rId62" display="@react-native-oh-tpl/react-native-autoheight-webview" tooltip="https://github.com/react-native-oh-library/react-native-autoheight-webview/releases"/>
-    <hyperlink ref="F49" r:id="rId3" location="/zh-cn/react-native-autoheight-webview" display="链接"/>
-    <hyperlink ref="B3" r:id="rId63" display="@react-native-camera-roll/camera-roll" tooltip="https://github.com/react-native-oh-library/react-native-cameraroll"/>
-    <hyperlink ref="E3" r:id="rId64" display="@react-native-oh-tpl/camera-roll" tooltip="https://github.com/react-native-oh-library/react-native-cameraroll/releases"/>
-    <hyperlink ref="F3" r:id="rId3" location="/zh-cn/react-native-cameraroll" display="链接"/>
-    <hyperlink ref="B11" r:id="rId65" display="@react-native-community/progress-view" tooltip="https://github.com/react-native-progress-view/progress-view"/>
-    <hyperlink ref="E11" r:id="rId66" display="@react-native-oh-tpl/progress-view" tooltip="https://github.com/react-native-oh-library/progress-view/releases"/>
-    <hyperlink ref="F11" r:id="rId3" location="/zh-cn/react-native-community-progress-view" display="链接"/>
-    <hyperlink ref="B18" r:id="rId67" display="@react-native-segmented-control/segmented-control" tooltip="https://github.com/react-native-segmented-control/segmented-control"/>
-    <hyperlink ref="F18" r:id="rId3" location="/zh-cn/react-native-community-segmented-control" display="链接"/>
-    <hyperlink ref="B56" r:id="rId68" display="react-native-dotenv" tooltip="https://github.com/goatandsheep/react-native-dotenv"/>
-    <hyperlink ref="F56" r:id="rId3" location="/zh-cn/react-native-dotenv" display="链接"/>
-    <hyperlink ref="B8" r:id="rId69" display="@react-native-community/geolocation" tooltip="https://github.com/michalchudziak/react-native-geolocation"/>
-    <hyperlink ref="E8" r:id="rId70" display="@react-native-oh-tpl/react-native-geolocation" tooltip="https://github.com/react-native-oh-library/react-native-geolocation/releases"/>
-    <hyperlink ref="F8" r:id="rId3" location="/zh-cn/react-native-geolocation" display="链接"/>
-    <hyperlink ref="B84" r:id="rId71" display="react-native-qrcode-svg" tooltip="https://github.com/awesomejerry/react-native-qrcode-svg"/>
-    <hyperlink ref="E84" r:id="rId72" display="@react-native-oh-tpl/react-native-qrcode-svg" tooltip="https://github.com/react-native-oh-library/react-native-qrcode-svg/releases"/>
-    <hyperlink ref="F84" r:id="rId3" location="/zh-cn/react-native-qrcode-svg" display="链接"/>
-    <hyperlink ref="B85" r:id="rId73" display="react-native-reanimated" tooltip="https://github.com/software-mansion/react-native-reanimated"/>
-    <hyperlink ref="E85" r:id="rId74" display="@react-native-oh-tpl/react-native-reanimated" tooltip="https://github.com/react-native-oh-library/react-native-reanimated/releases"/>
-    <hyperlink ref="F85" r:id="rId3" location="/zh-cn/react-native-reanimated" display="链接"/>
-    <hyperlink ref="B89" r:id="rId75" display="react-native-render-html" tooltip="https://github.com/meliorence/react-native-render-html"/>
-    <hyperlink ref="F89" r:id="rId3" location="/zh-cn/react-native-render-html" display="链接"/>
-    <hyperlink ref="B93" r:id="rId76" display="react-native-section-list-get-item-layout" tooltip="https://github.com/jsoendermann/rn-section-list-get-item-layout"/>
-    <hyperlink ref="F93" r:id="rId3" location="/zh-cn/react-native-section-list-get-item-layout" display="链接"/>
-    <hyperlink ref="B105" r:id="rId77" display="react-native-vector-icons" tooltip="https://github.com/oblador/react-native-vector-icons"/>
-    <hyperlink ref="F105" r:id="rId3" location="/zh-cn/react-native-vector-icons" display="链接"/>
-    <hyperlink ref="B107" r:id="rId78" display="react-native-view-shot" tooltip="https://github.com/gre/react-native-view-shot"/>
-    <hyperlink ref="E107" r:id="rId79" display="@react-native-oh-tpl/react-native-view-shot" tooltip="https://github.com/react-native-oh-library/react-native-view-shot/releases"/>
-    <hyperlink ref="F107" r:id="rId3" location="/zh-cn/react-native-view-shot" display="链接"/>
-    <hyperlink ref="B19" r:id="rId80" display="@react-navigation/bottom-tabs" tooltip="https://github.com/react-navigation/react-navigation/tree/6.x/packages/bottom-tabs"/>
-    <hyperlink ref="F19" r:id="rId3" location="/zh-cn/react-navigation-bottom-tabs" display="链接"/>
-    <hyperlink ref="B21" r:id="rId81" display="@react-navigation/native" tooltip="https://github.com/react-navigation/react-navigation/tree/6.x/packages/native"/>
-    <hyperlink ref="F21" r:id="rId3" location="/zh-cn/react-navigation-native" display="链接"/>
-    <hyperlink ref="B22" r:id="rId82" display="@react-navigation/stack" tooltip="https://github.com/react-navigation/react-navigation/tree/6.x/packages/stack"/>
-    <hyperlink ref="F22" r:id="rId3" location="/zh-cn/react-navigation-stack" display="链接"/>
-    <hyperlink ref="B113" r:id="rId83" display="recyclerlistview" tooltip="https://github.com/Flipkart/recyclerlistview"/>
-    <hyperlink ref="F113" r:id="rId3" location="/zh-cn/recyclerListView" display="链接"/>
-    <hyperlink ref="B120" r:id="rId84" display="rn-placeholder" tooltip="https://github.com/mfrachet/rn-placeholder"/>
-    <hyperlink ref="F120" r:id="rId85" display="链接"/>
-    <hyperlink ref="B121" r:id="rId86" display="styled-components" tooltip="https://github.com/styled-components/styled-components"/>
-    <hyperlink ref="F121" r:id="rId87" display="链接"/>
-    <hyperlink ref="B122" r:id="rId88" display="styled-system" tooltip="https://github.com/react-native-picker/picker"/>
-    <hyperlink ref="F122" r:id="rId89" display="链接"/>
-    <hyperlink ref="B31" r:id="rId90" display="jeanregisser/react-native-slider" tooltip="https://github.com/react-native-oh-library/jeanregisser-react-native-slider"/>
-    <hyperlink ref="F31" r:id="rId3" location="/zh-cn/jeanregisser-react-native-slider" display="链接"/>
-    <hyperlink ref="B34" r:id="rId53" display="js-beautify" tooltip="https://github.com/beautifier/js-beautify"/>
-    <hyperlink ref="F34" r:id="rId3" location="/zh-cn/js-beautify" display="链接"/>
-    <hyperlink ref="B50" r:id="rId91" display="react-native-base64" tooltip="https://github.com/eranbo/react-native-base64"/>
-    <hyperlink ref="F50" r:id="rId3" location="/zh-cn/react-native-base64" display="链接"/>
-    <hyperlink ref="B53" r:id="rId92" display="react-native-check-box" tooltip="https://github.com/crazycodeboy/react-native-check-box"/>
-    <hyperlink ref="F53" r:id="rId3" location="/zh-cn/react-native-check-box" display="链接"/>
-    <hyperlink ref="B5" r:id="rId93" display="@react-native-community/blur" tooltip="https://github.com/Kureev/react-native-blur"/>
-    <hyperlink ref="E5" r:id="rId94" display="@react-native-oh-tpl/blur Releases" tooltip="https://github.com/react-native-oh-library/react-native-blur/releases"/>
-    <hyperlink ref="F5" r:id="rId3" location="/zh-cn/react-native-community-blur" display="链接"/>
-    <hyperlink ref="B12" r:id="rId95" display="@react-native-community/push-notification-ios" tooltip="https://github.com/react-native-push-notification/ios"/>
-    <hyperlink ref="E12" r:id="rId96" display="@react-native-oh-tpl/push-notification-ios" tooltip="https://github.com/react-native-oh-library/react-native-push-notification-ios/releases"/>
-    <hyperlink ref="F12" r:id="rId3" location="/zh-cn/react-native-community-push-notification-ios" display="链接"/>
-    <hyperlink ref="B15" r:id="rId97" display="@react-native-cookies/cookies" tooltip="https://github.com/react-native-cookies/cookies"/>
-    <hyperlink ref="E15" r:id="rId98" display="@react-native-oh-tpl/cookies" tooltip="https://github.com/react-native-oh-library/react-native-cookies/releases"/>
-    <hyperlink ref="F15" r:id="rId3" location="/zh-cn/react-native-cookies" display="链接"/>
-    <hyperlink ref="B55" r:id="rId99" display="react-native-crypto-js" tooltip="https://github.com/imchintan/react-native-crypto-js"/>
-    <hyperlink ref="B73" r:id="rId100" display="react-native-maps" tooltip="https://github.com/react-native-maps/react-native-maps"/>
-    <hyperlink ref="E73" r:id="rId101" display="@react-native-oh-tpl/react-native-maps" tooltip="https://github.com/react-native-maps/react-native-maps/releases"/>
-    <hyperlink ref="F73" r:id="rId3" location="/zh-cn/react-native-maps" display="链接"/>
-    <hyperlink ref="B78" r:id="rId102" display="react-native-pdf" tooltip="https://github.com/wonday/react-native-pdf"/>
-    <hyperlink ref="E78" r:id="rId103" display="@react-native-oh-tpl/react-native-pdf" tooltip="https://github.com/react-native-oh-library/react-native-pdf/releases"/>
-    <hyperlink ref="F78" r:id="rId3" location="/zh-cn/react-native-pdf" display="链接"/>
-    <hyperlink ref="B88" r:id="rId104" display="react-native-redash" tooltip="https://github.com/wcandillon/react-native-redash/"/>
-    <hyperlink ref="F88" r:id="rId3" location="/zh-cn/react-native-redash" display="链接"/>
-    <hyperlink ref="B95" r:id="rId105" display="react-native-snap-carousel" tooltip="https://github.com/meliorence/react-native-snap-carousel"/>
-    <hyperlink ref="E95" r:id="rId106" display="@react-native-oh-tpl/react-native-snap-carousel" tooltip="https://github.com/react-native-oh-library/react-native-snap-carousel/releases"/>
-    <hyperlink ref="F95" r:id="rId3" location="/zh-cn/react-native-snap-carousel" display="链接"/>
-    <hyperlink ref="B103" r:id="rId107" display="react-native-transitiongroup" tooltip="https://github.com/madsleejensen/react-native-transitiongroup"/>
-    <hyperlink ref="E103" r:id="rId108" display="@react-native-oh-tpl/react-native-transitiongroup" tooltip="https://github.com/react-native-oh-library/react-native-transitiongroup/releases"/>
-    <hyperlink ref="F103" r:id="rId3" location="/zh-cn/react-native-transitiongroup" display="链接"/>
-    <hyperlink ref="B104" r:id="rId109" display="react-native-translucent-modal" tooltip="https://github.com/23mf/react-native-translucent-modal"/>
-    <hyperlink ref="E104" r:id="rId110" display="@react-native-oh-tpl/react-native-translucent-modal" tooltip="https://github.com/react-native-oh-library/react-native-translucent-modal/releases"/>
-    <hyperlink ref="F104" r:id="rId3" location="/zh-cn/react-native-translucent-modal" display="链接"/>
-    <hyperlink ref="B114" r:id="rId111" display="redux" tooltip="https://github.com/reduxjs/redux"/>
-    <hyperlink ref="F114" r:id="rId3" location="/zh-cn/redux" display="链接"/>
-    <hyperlink ref="B116" r:id="rId112" display="redux-logger" tooltip="https://github.com/LogRocket/redux-logger"/>
-    <hyperlink ref="F116" r:id="rId3" location="/zh-cn/redux-logger" display="链接"/>
-    <hyperlink ref="B117" r:id="rId113" display="redux-persist" tooltip="https://github.com/rt2zz/redux-persist"/>
-    <hyperlink ref="F117" r:id="rId3" location="/zh-cn/redux-persist" display="链接"/>
-    <hyperlink ref="B24" r:id="rId114" display="axios" tooltip="https://github.com/axios/axios"/>
-    <hyperlink ref="F24" r:id="rId3" location="/zh-cn/axios" display="链接"/>
-    <hyperlink ref="B26" r:id="rId115" display="dayJs" tooltip="https://github.com/iamkun/dayjs?tab=readme-ov-file"/>
-    <hyperlink ref="F26" r:id="rId3" location="/zh-cn/dayjs" display="链接"/>
-    <hyperlink ref="B28" r:id="rId116" display="EventBus" tooltip="https://github.com/krasimir/EventBus"/>
-    <hyperlink ref="F28" r:id="rId3" location="/zh-cn/EventBus" display="链接"/>
-    <hyperlink ref="B30" r:id="rId117" display="immer" tooltip="https://github.com/immerjs/immer"/>
-    <hyperlink ref="F30" r:id="rId3" location="/zh-cn/immer" display="链接"/>
-    <hyperlink ref="B32" r:id="rId118" display="JsBarCode" tooltip="https://github.com/lindell/JsBarcode"/>
-    <hyperlink ref="F32" r:id="rId3" location="/zh-cn/jsbarcode" display="链接"/>
-    <hyperlink ref="B39" r:id="rId119" display="Moment" tooltip="https://github.com/moment/moment"/>
-    <hyperlink ref="F39" r:id="rId3" location="/zh-cn/moment" display="链接"/>
-    <hyperlink ref="B42" r:id="rId120" display="qrcode-generator" tooltip="https://github.com/kazuhikoarase/qrcode-generator"/>
-    <hyperlink ref="F42" r:id="rId3" location="/zh-cn/qrcode-generator" display="链接"/>
-    <hyperlink ref="B43" r:id="rId121" display="react-ahooks" tooltip="https://github.com/alibaba/hooks"/>
-    <hyperlink ref="F43" r:id="rId3" location="/zh-cn/react-ahooks" display="链接"/>
-    <hyperlink ref="B45" r:id="rId122" display="react-lifecycles-compat" tooltip="https://github.com/reactjs/react-lifecycles-compat"/>
-    <hyperlink ref="F45" r:id="rId3" location="/zh-cn/react-lifecycles-compat" display="链接"/>
-    <hyperlink ref="B47" r:id="rId123" display="react-native-animate-number" tooltip="https://github.com/wkh237/react-native-animate-number"/>
-    <hyperlink ref="F47" r:id="rId3" location="/zh-cn/react-native-animate-number" display="链接"/>
-    <hyperlink ref="B51" r:id="rId124" display="react-native-blob-util" tooltip="https://github.com/react-native-oh-library/react-native-blob-util"/>
-    <hyperlink ref="E51" r:id="rId125" display="@react-native-oh-tpl/react-native-blob-util" tooltip="https://github.com/react-native-oh-library/react-native-blob-util/releases"/>
-    <hyperlink ref="F51" r:id="rId3" location="/zh-cn/react-native-blob-util" display="链接"/>
-    <hyperlink ref="B52" r:id="rId126" display="react-native-canvas" tooltip="https://github.com/iddan/react-native-canvas"/>
-    <hyperlink ref="F52" r:id="rId3" location="/zh-cn/react-native-canvas" display="链接"/>
-    <hyperlink ref="B54" r:id="rId127" display="react-native-confirmation-code-field" tooltip="https://github.com/retyui/react-native-confirmation-code-field"/>
-    <hyperlink ref="F54" r:id="rId3" location="/zh-cn/react-native-confirmation-code-field" display="链接"/>
-    <hyperlink ref="B58" r:id="rId128" display="react-native-drawer-layout-polyfill" tooltip="https://github.com/rnc-archive/react-native-drawer-layout-polyfill"/>
-    <hyperlink ref="F58" r:id="rId3" location="/zh-cn/react-native-drawer-layout-polyfill" display="链接"/>
-    <hyperlink ref="B59" r:id="rId129" display="react-native-echarts-pro" tooltip="https://github.com/supervons/react-native-echarts-pro"/>
-    <hyperlink ref="F59" r:id="rId3" location="/zh-cn/react-native-echarts-pro" display="链接"/>
-    <hyperlink ref="B62" r:id="rId130" display="react-native-fit-Image" tooltip="https://github.com/huiseoul/react-native-fit-image"/>
-    <hyperlink ref="E62" r:id="rId131" display="@react-native-oh-tpl/react-native-fit-Image" tooltip="https://github.com/huiseoul/react-native-fit-image/releases"/>
-    <hyperlink ref="F62" r:id="rId3" location="/zh-cn/react-native-fit-Image" display="链接"/>
-    <hyperlink ref="B65" r:id="rId132" display="react-native-image-editor" tooltip="https://github.com/react-native-oh-library/react-native-image-editor"/>
-    <hyperlink ref="E65" r:id="rId133" display="@react-native-oh-tpl/react-native-image-editor" tooltip="https://github.com/react-native-oh-library/react-native-image-editor/releases"/>
-    <hyperlink ref="F65" r:id="rId3" location="/zh-cn/react-native-image-editor" display="链接"/>
-    <hyperlink ref="B67" r:id="rId134" display="react-native-image-viewer" tooltip="https://github.com/react-native-oh-library/react-native-image-viewer"/>
-    <hyperlink ref="E67" r:id="rId135" display="react-native-image-viewer" tooltip="https://github.com/react-native-oh-library/react-native-image-viewer/releases"/>
-    <hyperlink ref="F67" r:id="rId3" location="/zh-cn/react-native-image-viewer" display="链接"/>
-    <hyperlink ref="B69" r:id="rId136" display="react-native-image-zoom" tooltip="https://github.com/react-native-oh-library/react-native-image-zoom"/>
-    <hyperlink ref="E69" r:id="rId137" display="@react-native-oh-tpl/react-native-image-zoom" tooltip="https://github.com/react-native-oh-library/react-native-image-zoom/releases"/>
-    <hyperlink ref="F69" r:id="rId3" location="/zh-cn/react-native-image-zoom" display="链接"/>
-    <hyperlink ref="B70" r:id="rId138" display="react-native-intersection-observer" tooltip="https://github.com/react-native-oh-library/react-native-intersection-observer"/>
-    <hyperlink ref="E70" r:id="rId139" display="@react-native-oh-tpl/react-native-intersection-observer" tooltip="https://github.com/react-native-oh-library/react-native-intersection-observer/releases"/>
-    <hyperlink ref="F70" r:id="rId3" location="/zh-cn/react-native-intersection-observer" display="链接"/>
-    <hyperlink ref="B68" r:id="rId140" display="react-native-image-viewing" tooltip="https://github.com/react-native-oh-library/react-native-image-viewing"/>
-    <hyperlink ref="E68" r:id="rId141" display="@react-native-oh-tpl/react-native-image-viewing" tooltip="https://github.com/react-native-oh-library/react-native-image-viewing/releases"/>
-    <hyperlink ref="F68" r:id="rId3" location="/zh-cn/react-native-image-viewing" display="链接"/>
-    <hyperlink ref="B74" r:id="rId142" display="react-native-markdown-display" tooltip="https://github.com/react-native-oh-library/react-native-markdown-display/tree/sig"/>
-    <hyperlink ref="E74" r:id="rId143" display="@react-native-oh-tpl/react-native-markdown-display" tooltip="https://github.com/react-native-oh-library/react-native-markdown-display/releases"/>
-    <hyperlink ref="F74" r:id="rId3" location="/zh-cn/react-native-markdown-display" display="链接"/>
-    <hyperlink ref="B75" r:id="rId144" display="react-native-marquee" tooltip="https://github.com/react-native-oh-library/react-native-marquee"/>
-    <hyperlink ref="E75" r:id="rId145" display="@react-native-oh-tpl/react-native-marquee" tooltip="https://github.com/react-native-oh-library/react-native-marquee/releases"/>
-    <hyperlink ref="F75" r:id="rId3" location="/zh-cn/react-native-marquee" display="链接"/>
-    <hyperlink ref="B80" r:id="rId146" display="react-native-popover-view" tooltip="https://github.com/react-native-oh-library/react-native-popover-view"/>
-    <hyperlink ref="E80" r:id="rId147" display="@react-native-oh-tpl/react-native-popover-view" tooltip="https://github.com/react-native-oh-library/react-native-popover-view/releases"/>
-    <hyperlink ref="F80" r:id="rId3" location="/zh-cn/react-native-popover-view" display="链接"/>
-    <hyperlink ref="B81" r:id="rId148" display="react-native-popup-menu" tooltip="https://github.com/instea/react-native-popup-menu"/>
-    <hyperlink ref="F81" r:id="rId3" location="/zh-cn/react-native-popup-menu" display="链接"/>
-    <hyperlink ref="B83" r:id="rId149" display="react-native-pull" tooltip="https://github.com/react-native-oh-library/react-native-pull"/>
-    <hyperlink ref="E83" r:id="rId150" display="@react-native-oh-tpl/react-native-pull" tooltip="https://github.com/react-native-oh-library/react-native-pull/releases"/>
-    <hyperlink ref="F83" r:id="rId3" location="/zh-cn/react-native-pull" display="链接"/>
-    <hyperlink ref="B87" r:id="rId151" display="react-native-reanimated-table" tooltip="https://github.com/dohooo/react-native-reanimated-table"/>
-    <hyperlink ref="F87" r:id="rId3" location="/zh-cn/react-native-reanimated-table" display="链接"/>
-    <hyperlink ref="B92" r:id="rId152" display="react-native-scrollable-tab-view" tooltip="https://github.com/react-native-oh-library/react-native-scrollable-tab-view"/>
-    <hyperlink ref="F92" r:id="rId3" location="/zh-cn/react-native-scrollable-tab-view" display="链接"/>
-    <hyperlink ref="B97" r:id="rId153" display="react-native-stickyheader" tooltip="https://github.com/react-native-oh-library/react-native-stickyheader"/>
-    <hyperlink ref="E97" r:id="rId154" display="@react-native-oh-tpl/react-native-stickyheader" tooltip="https://github.com/react-native-oh-library/react-native-stickyheader/releases"/>
-    <hyperlink ref="F97" r:id="rId3" location="/zh-cn/react-native-stickyheader" display="链接"/>
-    <hyperlink ref="B99" r:id="rId128" display="react-native-swipe-list-view" tooltip="https://github.com/rnc-archive/react-native-drawer-layout-polyfill"/>
-    <hyperlink ref="F99" r:id="rId3" location="/zh-cn/react-native-swipe-list-view" display="链接"/>
-    <hyperlink ref="B100" r:id="rId155" display="react-native-swiper" tooltip="https://github.com/leecade/react-native-swiper"/>
-    <hyperlink ref="F100" r:id="rId3" location="/zh-cn/react-native-swiper" display="链接"/>
-    <hyperlink ref="B109" r:id="rId156" display="react-native-worklets-core" tooltip="https://github.com/react-native-oh-library/react-native-worklets-core"/>
-    <hyperlink ref="E109" r:id="rId157" display="@react-native-oh-tpl/react-native-worklets-core" tooltip="https://github.com/react-native-oh-library/react-native-worklets-core/releases"/>
-    <hyperlink ref="F109" r:id="rId3" location="/zh-cn/react-native-worklets-core" display="链接"/>
-    <hyperlink ref="B112" r:id="rId158" display="react-use" tooltip="https://github.com/zenghongtu/react-use"/>
-    <hyperlink ref="F112" r:id="rId3" location="/zh-cn/react-use" display="链接"/>
-    <hyperlink ref="B119" r:id="rId159" display="redux-toolkit" tooltip="https://github.com/reduxjs/redux-toolkit"/>
-    <hyperlink ref="F119" r:id="rId160" display="链接"/>
-    <hyperlink ref="B102" r:id="rId161" display="react-native-text-size" tooltip="https://github.com/aMarCruz/react-native-text-size"/>
-    <hyperlink ref="E102" r:id="rId162" display="@react-native-oh-tpl/react-native-text-size" tooltip="https://github.com/react-native-oh-library/react-native-text-size/releases"/>
-    <hyperlink ref="F102" r:id="rId3" location="/zh-cn/react-native-text-size" display="链接"/>
-    <hyperlink ref="B111" r:id="rId163" display="react-router-dom" tooltip="https://github.com/remix-run/react-router"/>
-    <hyperlink ref="F111" r:id="rId3" location="/zh-cn/react-router-dom" display="链接"/>
-    <hyperlink ref="B115" r:id="rId164" display="redux-actions" tooltip="https://github.com/redux-utilities/redux-actions"/>
-    <hyperlink ref="F115" r:id="rId3" location="/zh-cn/redux-actions" display="链接"/>
-    <hyperlink ref="B118" r:id="rId165" display="redux-thunk" tooltip="https://github.com/reduxjs/redux-thunk"/>
-    <hyperlink ref="F118" r:id="rId3" location="/zh-cn/redux-thunk" display="链接"/>
-    <hyperlink ref="B48" r:id="rId166" display="react-native-aria" tooltip="https://github.com/gluestack/react-native-aria/"/>
-    <hyperlink ref="F48" r:id="rId3" location="/zh-cn/react-native-aria" display="链接"/>
-    <hyperlink ref="B82" r:id="rId167" display="react-native-progress" tooltip="https://github.com/oblador/react-native-progress"/>
-    <hyperlink ref="E82" r:id="rId168" display="@react-native-oh-tpl/react-native-progress" tooltip="https://github.com/react-native-oh-library/react-native-progress/releases"/>
-    <hyperlink ref="F82" r:id="rId3" location="/zh-cn/react-native-progress" display="链接"/>
-    <hyperlink ref="B63" r:id="rId169" display="react-native-fs" tooltip="https://github.com/itinance/react-native-fs"/>
-    <hyperlink ref="E63" r:id="rId170" display="@react-native-oh-tpl/react-native-fs" tooltip="https://github.com/react-native-oh-library/react-native-fs/releases"/>
-    <hyperlink ref="F63" r:id="rId3" location="/zh-cn/react-native-fs" display="链接"/>
-    <hyperlink ref="B71" r:id="rId171" display="react-native-keyboard-aware-scroll-view" tooltip="https://github.com/APSL/react-native-keyboard-aware-scroll-view"/>
-    <hyperlink ref="E71" r:id="rId172" display="@react-native-oh-tpl/react-native-keyboard-aware-scroll-view" tooltip="https://github.com/react-native-oh-library/react-native-keyboard-aware-scroll-view/releases"/>
-    <hyperlink ref="F71" r:id="rId3" location="/zh-cn/react-native-keyboard-aware-scroll-view" display="链接"/>
-    <hyperlink ref="B79" r:id="rId173" display="react-native-permissions" tooltip="https://github.com/zoontek/react-native-permissions"/>
-    <hyperlink ref="E79" r:id="rId174" display="@react-native-oh-tpl/react-native-permissions" tooltip="https://github.com/react-native-oh-library/react-native-permissions/releases"/>
-    <hyperlink ref="F79" r:id="rId3" location="/zh-cn/react-native-permissions" display="链接"/>
-    <hyperlink ref="B57" r:id="rId175" display="react-native-drag-sort" tooltip="https://github.com/mochixuan/react-native-drag-sort"/>
-    <hyperlink ref="F57" r:id="rId3" location="/zh-cn/react-native-drag-sort" display="链接"/>
-    <hyperlink ref="B96" r:id="rId176" display="react-native-sound" tooltip="https://github.com/zmxv/react-native-sound"/>
-    <hyperlink ref="E96" r:id="rId177" display="@react-native-oh-tpl/react-native-sound" tooltip="https://github.com/react-native-oh-library/react-native-sound/releases"/>
-    <hyperlink ref="F96" r:id="rId3" location="/zh-cn/react-native-sound" display="链接"/>
-    <hyperlink ref="B86" r:id="rId178" display="react-native-reanimated-carousel" tooltip="https://github.com/dohooo/react-native-reanimated-carousel"/>
-    <hyperlink ref="F86" r:id="rId3" location="/zh-cn/react-native-reanimated-carousel" display="链接"/>
-    <hyperlink ref="B14" r:id="rId179" display="@react-native-community/toolbar-android" tooltip="https://github.com/react-native-toolbar-android/toolbar-android"/>
-    <hyperlink ref="E14" r:id="rId180" display="@react-native-oh-tpl/toolbar-android" tooltip="https://github.com/react-native-oh-library/toolbar-android/releases"/>
-    <hyperlink ref="F14" r:id="rId3" location="/zh-cn/react-native-toolbar-android" display="链接"/>
-    <hyperlink ref="B110" r:id="rId181" display="react-redux" tooltip="https://github.com/reduxjs/react-redux"/>
-    <hyperlink ref="F110" r:id="rId3" location="/zh-cn/react-redux" display="链接"/>
-    <hyperlink ref="B76" r:id="rId182" display="react-native-MJRefresh" tooltip="https://github.com/react-native-studio/react-native-MJRefresh"/>
-    <hyperlink ref="E76" r:id="rId183" display="@react-native-oh-tpl/react-native-mjrefresh" tooltip="https://github.com/react-native-oh-library/react-native-MJRefresh/releases"/>
-    <hyperlink ref="E92" r:id="rId184" display="@react-native-oh-tpl/react-native-scrollable-tab-view" tooltip="https://github.com/react-native-oh-library/react-native-scrollable-tab-view/releases"/>
-    <hyperlink ref="F55" r:id="rId3" location="/zh-cn/react-native-crypto-js" display="链接"/>
-    <hyperlink ref="F76" r:id="rId3" location="/zh-cn/react-native-MJRefresh" display="链接"/>
-    <hyperlink ref="F123" r:id="rId185" display="链接"/>
-    <hyperlink ref="F124" r:id="rId186" display="链接"/>
-    <hyperlink ref="E124" r:id="rId187" display="@react-native-oh-tpl/react-native-sortable-list"/>
-    <hyperlink ref="B124" r:id="rId188" display="react-native-sortable-list"/>
-    <hyperlink ref="B123" r:id="rId189" display="react-native-sensors"/>
-    <hyperlink ref="E123" r:id="rId190" display="@react-native-oh-tpl/react-native-sensors"/>
-    <hyperlink ref="B126" r:id="rId191" display="react-native-image-sequence-2"/>
-    <hyperlink ref="E126" r:id="rId192" display="@react-native-oh-tpl/react-native-image-sequence-2"/>
-    <hyperlink ref="F126" r:id="rId3" location="/zh-cn/react-native-sequence-2" display="链接"/>
-    <hyperlink ref="B127" r:id="rId193" display="react-native-feather"/>
-    <hyperlink ref="F127" r:id="rId3" location="/zh-cn/react-native-feather" display="链接"/>
-    <hyperlink ref="B125" r:id="rId194" display="react-native-easy-toast"/>
-    <hyperlink ref="F125" r:id="rId3" location="/zh-cn/react-native-sequence-2" display="链接"/>
-    <hyperlink ref="B128" r:id="rId195" display="@react-navigation/native-stack"/>
-    <hyperlink ref="E128" r:id="rId196" display="@react-native-oh-tpl/native-stack"/>
-    <hyperlink ref="F128" r:id="rId3" location="/zh-cn/react-navigation-native-stack.md" display="链接"/>
-    <hyperlink ref="B129" r:id="rId197" display="react-native-waterfall-flow"/>
-    <hyperlink ref="F129" r:id="rId198" display="链接"/>
-    <hyperlink ref="B130" r:id="rId199" display="react-native-vconsole"/>
-    <hyperlink ref="F130" r:id="rId200" display="链接"/>
-    <hyperlink ref="B131" r:id="rId201" display="better-banner"/>
-    <hyperlink ref="F131" r:id="rId202" display="链接"/>
-    <hyperlink ref="B132" r:id="rId203" display="react-native-ezswiper"/>
-    <hyperlink ref="F132" r:id="rId204" display="链接"/>
-    <hyperlink ref="B133" r:id="rId205" display="react-native-image-header-scroll-view"/>
-    <hyperlink ref="F133" r:id="rId206" display="链接"/>
-    <hyperlink ref="B134" r:id="rId207" display="react-native-linear-gradient-text"/>
-    <hyperlink ref="F134" r:id="rId208" display="链接"/>
-    <hyperlink ref="B135" r:id="rId209" display="react-native-marquee-ab"/>
-    <hyperlink ref="F135" r:id="rId210" display="链接"/>
-    <hyperlink ref="B136" r:id="rId211" display="react-native-reconnecting-websocket"/>
-    <hyperlink ref="F136" r:id="rId212" display="链接"/>
-    <hyperlink ref="B137" r:id="rId213" display="react-native-json-tree"/>
-    <hyperlink ref="F137" r:id="rId214" display="链接"/>
-    <hyperlink ref="B138" r:id="rId215" display="react-native-image-gallery"/>
-    <hyperlink ref="F138" r:id="rId216" display="链接"/>
-    <hyperlink ref="E138" r:id="rId217" display="@react-native-oh-tpl/react-native-image-gallery"/>
+    <hyperlink ref="F4" r:id="rId6" display="链接"/>
+    <hyperlink ref="B7" r:id="rId7" display="@react-native-community/datetimepicker" tooltip="https://github.com/react-native-datetimepicker/datetimepicker"/>
+    <hyperlink ref="E7" r:id="rId8" display="@react-native-oh-tpl/datetimepicker" tooltip="https://github.com/react-native-oh-library/datetimepicker/releases"/>
+    <hyperlink ref="F7" r:id="rId9" display="链接"/>
+    <hyperlink ref="B23" r:id="rId10" display="@shopify/flash-list" tooltip="https://github.com/Shopify/flash-list"/>
+    <hyperlink ref="E23" r:id="rId11" display="@react-native-oh-tpl/flash-list" tooltip="https://github.com/react-native-oh-library/flash-list/releases"/>
+    <hyperlink ref="F23" r:id="rId12" display="链接"/>
+    <hyperlink ref="B36" r:id="rId13" display="lottie-react-native" tooltip="https://github.com/lottie-react-native/lottie-react-native"/>
+    <hyperlink ref="E36" r:id="rId14" display="@react-native-oh-tpl/lottie-react-native" tooltip="https://github.com/react-native-oh-library/lottie-react-native/releases"/>
+    <hyperlink ref="F36" r:id="rId15" display="链接"/>
+    <hyperlink ref="B17" r:id="rId16" display="@react-native-picker/picker" tooltip="https://github.com/react-native-picker/picker"/>
+    <hyperlink ref="E17" r:id="rId17" display="@react-native-oh-tpl/picker" tooltip="https://github.com/react-native-oh-library/picker/releases"/>
+    <hyperlink ref="F17" r:id="rId18" display="链接"/>
+    <hyperlink ref="B10" r:id="rId19" display="@react-native-community/progress-bar-android" tooltip="https://github.com/react-native-progress-view/progress-bar-android"/>
+    <hyperlink ref="E10" r:id="rId20" display="@react-native-oh-tpl/progress-bar-android" tooltip="https://github.com/react-native-oh-library/progress-bar-android/releases"/>
+    <hyperlink ref="F10" r:id="rId21" display="链接"/>
+    <hyperlink ref="B6" r:id="rId22" display="@react-native-community/checkbox" tooltip="https://github.com/react-native-checkbox/react-native-checkbox"/>
+    <hyperlink ref="E6" r:id="rId23" display="@react-native-oh-tpl/react-native-checkbox" tooltip="https://github.com/react-native-oh-library/react-native-checkbox/releases"/>
+    <hyperlink ref="F6" r:id="rId24" display="链接"/>
+    <hyperlink ref="B60" r:id="rId25" display="react-native-exception-handler" tooltip="https://github.com/a7ul/react-native-exception-handler"/>
+    <hyperlink ref="E60" r:id="rId26" display="@react-native-oh-tpl/react-native-exception-handler" tooltip="https://github.com/react-native-oh-library/react-native-exception-handler/releases"/>
+    <hyperlink ref="F60" r:id="rId27" display="链接"/>
+    <hyperlink ref="B61" r:id="rId28" display="react-native-fast-image" tooltip="https://github.com/DylanVann/react-native-fast-image"/>
+    <hyperlink ref="E61" r:id="rId29" display="@react-native-oh-tpl/react-native-fast-image" tooltip="https://github.com/react-native-oh-library/react-native-fast-image/releases"/>
+    <hyperlink ref="F61" r:id="rId30" display="链接"/>
+    <hyperlink ref="B64" r:id="rId31" display="react-native-gesture-handler" tooltip="https://github.com/software-mansion/react-native-gesture-handler"/>
+    <hyperlink ref="E64" r:id="rId32" display="@react-native-oh-tpl/react-native-gesture-handler" tooltip="https://github.com/react-native-oh-library/react-native-gesture-handler/releases"/>
+    <hyperlink ref="F64" r:id="rId33" display="链接"/>
+    <hyperlink ref="B66" r:id="rId34" display="react-native-image-picker" tooltip="https://github.com/react-native-image-picker/react-native-image-picker"/>
+    <hyperlink ref="E66" r:id="rId35" display="@react-native-oh-tpl/react-native-image-picker" tooltip="https://github.com/react-native-oh-library/react-native-image-picker/releases"/>
+    <hyperlink ref="F66" r:id="rId36" display="链接"/>
+    <hyperlink ref="B72" r:id="rId37" display="react-native-linear-gradient" tooltip="https://github.com/react-native-linear-gradient/react-native-linear-gradient"/>
+    <hyperlink ref="E72" r:id="rId38" display="@react-native-oh-tpl/react-native-linear-gradient" tooltip="https://github.com/react-native-oh-library/react-native-linear-gradient/releases"/>
+    <hyperlink ref="F72" r:id="rId39" display="链接"/>
+    <hyperlink ref="B16" r:id="rId40" display="@react-native-masked-view/masked-view" tooltip="https://github.com/react-native-masked-view/masked-view"/>
+    <hyperlink ref="E16" r:id="rId41" display="@react-native-oh-tpl/masked-view" tooltip="https://github.com/react-native-oh-library/masked-view/releases"/>
+    <hyperlink ref="F16" r:id="rId42" display="链接"/>
+    <hyperlink ref="B9" r:id="rId43" display="@react-native-community/netinfo" tooltip="https://github.com/react-native-netinfo/react-native-netinfo"/>
+    <hyperlink ref="E9" r:id="rId44" display="@react-native-oh-tpl/netinfo" tooltip="https://github.com/react-native-oh-library/react-native-netinfo/releases"/>
+    <hyperlink ref="F9" r:id="rId45" display="链接"/>
+    <hyperlink ref="B77" r:id="rId46" display="react-native-pager-view" tooltip="https://github.com/callstack/react-native-pager-view"/>
+    <hyperlink ref="E77" r:id="rId47" display="@react-native-oh-tpl/react-native-pager-view" tooltip="https://github.com/react-native-oh-library/react-native-pager-view/releases"/>
+    <hyperlink ref="F77" r:id="rId48" display="链接"/>
+    <hyperlink ref="B90" r:id="rId49" display="react-native-safe-area-context" tooltip="https://github.com/th3rdwave/react-native-safe-area-context"/>
+    <hyperlink ref="E90" r:id="rId50" display="@react-native-oh-tpl/react-native-safe-area-context" tooltip="https://github.com/react-native-oh-library/react-native-safe-area-context/releases"/>
+    <hyperlink ref="F90" r:id="rId51" display="链接"/>
+    <hyperlink ref="B91" r:id="rId52" display="react-native-screens" tooltip="https://github.com/software-mansion/react-native-screens"/>
+    <hyperlink ref="F91" r:id="rId53" display="链接"/>
+    <hyperlink ref="B13" r:id="rId54" display="@react-native-community/slider" tooltip="https://github.com/callstack/react-native-slider"/>
+    <hyperlink ref="E13" r:id="rId55" display="@react-native-oh-tpl/slider" tooltip="https://github.com/react-native-oh-library/react-native-slider/releases"/>
+    <hyperlink ref="F13" r:id="rId56" display="链接"/>
+    <hyperlink ref="B94" r:id="rId57" display="react-native-SmartRefreshLayout" tooltip="https://github.com/react-native-studio/react-native-SmartRefreshLayout"/>
+    <hyperlink ref="E94" r:id="rId58" display="@react-native-oh-tpl/react-native-SmartRefreshLayout" tooltip="https://github.com/react-native-oh-library/react-native-SmartRefreshLayout/releases"/>
+    <hyperlink ref="F94" r:id="rId59" display="链接"/>
+    <hyperlink ref="B98" r:id="rId60" display="react-native-svg" tooltip="https://github.com/software-mansion/react-native-svg"/>
+    <hyperlink ref="E98" r:id="rId61" display="@react-native-oh-tpl/react-native-svg" tooltip="https://github.com/react-native-oh-library/react-native-svg/releases"/>
+    <hyperlink ref="F98" r:id="rId62" display="链接"/>
+    <hyperlink ref="B101" r:id="rId63" display="react-native-tab-view" tooltip="https://github.com/react-navigation/react-navigation/tree/6.x/packages/react-native-tab-view"/>
+    <hyperlink ref="E101" r:id="rId64" display="@react-native-oh-tpl/react-native-tab-view" tooltip="https://github.com/react-native-oh-library/react-navigation/releases"/>
+    <hyperlink ref="F101" r:id="rId65" display="链接"/>
+    <hyperlink ref="B106" r:id="rId66" display="react-native-video" tooltip="https://github.com/react-native-video/react-native-video"/>
+    <hyperlink ref="E106" r:id="rId67" display="@react-native-oh-tpl/react-native-video" tooltip="https://github.com/react-native-oh-library/react-native-video"/>
+    <hyperlink ref="F106" r:id="rId68" display="链接"/>
+    <hyperlink ref="B108" r:id="rId69" display="react-native-webview" tooltip="https://github.com/react-native-webview/react-native-webview"/>
+    <hyperlink ref="E108" r:id="rId70" display="@react-native-oh-tpl/react-native-webview" tooltip="https://github.com/react-native-oh-library/react-native-webview/releases"/>
+    <hyperlink ref="F108" r:id="rId71" display="链接"/>
+    <hyperlink ref="B20" r:id="rId72" display="@react-navigation/elements" tooltip="https://github.com/react-navigation/react-navigation/tree/6.x/packages/elements"/>
+    <hyperlink ref="E20" r:id="rId64" display="@react-native-oh-tpl/elements" tooltip="https://github.com/react-native-oh-library/react-navigation/releases"/>
+    <hyperlink ref="F20" r:id="rId73" display="链接"/>
+    <hyperlink ref="B25" r:id="rId74" display="crypto-js" tooltip="https://github.com/brix/crypto-js/tree/4.2.0"/>
+    <hyperlink ref="F25" r:id="rId75" display="链接"/>
+    <hyperlink ref="B27" r:id="rId76" display="deepmerge" tooltip="https://github.com/TehShrike/deepmerge"/>
+    <hyperlink ref="F27" r:id="rId77" display="链接"/>
+    <hyperlink ref="B29" r:id="rId78" display="htmlparser2" tooltip="https://github.com/fb55/htmlparser2"/>
+    <hyperlink ref="F29" r:id="rId79" display="链接"/>
+    <hyperlink ref="B33" r:id="rId80" display="js-beautify" tooltip="https://github.com/beautifier/js-beautify"/>
+    <hyperlink ref="F33" r:id="rId81" display="链接"/>
+    <hyperlink ref="B35" r:id="rId82" display="lodash" tooltip="https://github.com/lodash/lodash/tree/4.17.21"/>
+    <hyperlink ref="F35" r:id="rId83" display="链接"/>
+    <hyperlink ref="B38" r:id="rId84" display="mobx-react" tooltip="https://github.com/mobxjs/mobx/tree/mobx-react@7.6.0"/>
+    <hyperlink ref="F38" r:id="rId85" display="链接"/>
+    <hyperlink ref="B37" r:id="rId86" display="mobx" tooltip="https://github.com/mobxjs/mobx/tree/mobx@6.10.0"/>
+    <hyperlink ref="F37" r:id="rId87" display="链接"/>
+    <hyperlink ref="B40" r:id="rId88" display="parse5" tooltip="https://github.com/inikulin/parse5"/>
+    <hyperlink ref="F40" r:id="rId89" display="链接"/>
+    <hyperlink ref="B41" r:id="rId90" display="prop-types" tooltip="https://github.com/facebook/prop-types/tree/v15.8.1"/>
+    <hyperlink ref="F41" r:id="rId91" display="链接"/>
+    <hyperlink ref="B44" r:id="rId92" display="react-i18next" tooltip="https://github.com/i18next/react-i18next"/>
+    <hyperlink ref="F44" r:id="rId93" display="链接"/>
+    <hyperlink ref="B46" r:id="rId94" display="react-native-action-button" tooltip="https://github.com/mastermoo/react-native-action-button"/>
+    <hyperlink ref="F46" r:id="rId95" display="链接"/>
+    <hyperlink ref="B49" r:id="rId96" display="react-native-autoheight-webview" tooltip="https://github.com/react-native-oh-library/react-native-autoheight-webview"/>
+    <hyperlink ref="E49" r:id="rId97" display="@react-native-oh-tpl/react-native-autoheight-webview" tooltip="https://github.com/react-native-oh-library/react-native-autoheight-webview/releases"/>
+    <hyperlink ref="F49" r:id="rId98" display="链接"/>
+    <hyperlink ref="B3" r:id="rId99" display="@react-native-camera-roll/camera-roll" tooltip="https://github.com/react-native-oh-library/react-native-cameraroll"/>
+    <hyperlink ref="E3" r:id="rId100" display="@react-native-oh-tpl/camera-roll" tooltip="https://github.com/react-native-oh-library/react-native-cameraroll/releases"/>
+    <hyperlink ref="F3" r:id="rId101" display="链接"/>
+    <hyperlink ref="B11" r:id="rId102" display="@react-native-community/progress-view" tooltip="https://github.com/react-native-progress-view/progress-view"/>
+    <hyperlink ref="E11" r:id="rId103" display="@react-native-oh-tpl/progress-view" tooltip="https://github.com/react-native-oh-library/progress-view/releases"/>
+    <hyperlink ref="F11" r:id="rId104" display="链接"/>
+    <hyperlink ref="B18" r:id="rId105" display="@react-native-segmented-control/segmented-control" tooltip="https://github.com/react-native-segmented-control/segmented-control"/>
+    <hyperlink ref="F18" r:id="rId106" display="链接"/>
+    <hyperlink ref="B56" r:id="rId107" display="react-native-dotenv" tooltip="https://github.com/goatandsheep/react-native-dotenv"/>
+    <hyperlink ref="F56" r:id="rId108" display="链接"/>
+    <hyperlink ref="B8" r:id="rId109" display="@react-native-community/geolocation" tooltip="https://github.com/michalchudziak/react-native-geolocation"/>
+    <hyperlink ref="E8" r:id="rId110" display="@react-native-oh-tpl/react-native-geolocation" tooltip="https://github.com/react-native-oh-library/react-native-geolocation/releases"/>
+    <hyperlink ref="F8" r:id="rId111" display="链接"/>
+    <hyperlink ref="B84" r:id="rId112" display="react-native-qrcode-svg" tooltip="https://github.com/awesomejerry/react-native-qrcode-svg"/>
+    <hyperlink ref="E84" r:id="rId113" display="@react-native-oh-tpl/react-native-qrcode-svg" tooltip="https://github.com/react-native-oh-library/react-native-qrcode-svg/releases"/>
+    <hyperlink ref="F84" r:id="rId114" display="链接"/>
+    <hyperlink ref="B85" r:id="rId115" display="react-native-reanimated" tooltip="https://github.com/software-mansion/react-native-reanimated"/>
+    <hyperlink ref="E85" r:id="rId116" display="@react-native-oh-tpl/react-native-reanimated" tooltip="https://github.com/react-native-oh-library/react-native-reanimated/releases"/>
+    <hyperlink ref="F85" r:id="rId117" display="链接"/>
+    <hyperlink ref="B89" r:id="rId118" display="react-native-render-html" tooltip="https://github.com/meliorence/react-native-render-html"/>
+    <hyperlink ref="F89" r:id="rId119" display="链接"/>
+    <hyperlink ref="B93" r:id="rId120" display="react-native-section-list-get-item-layout" tooltip="https://github.com/jsoendermann/rn-section-list-get-item-layout"/>
+    <hyperlink ref="F93" r:id="rId121" display="链接"/>
+    <hyperlink ref="B105" r:id="rId122" display="react-native-vector-icons" tooltip="https://github.com/oblador/react-native-vector-icons"/>
+    <hyperlink ref="F105" r:id="rId123" display="链接"/>
+    <hyperlink ref="B107" r:id="rId124" display="react-native-view-shot" tooltip="https://github.com/gre/react-native-view-shot"/>
+    <hyperlink ref="E107" r:id="rId125" display="@react-native-oh-tpl/react-native-view-shot" tooltip="https://github.com/react-native-oh-library/react-native-view-shot/releases"/>
+    <hyperlink ref="F107" r:id="rId126" display="链接"/>
+    <hyperlink ref="B19" r:id="rId127" display="@react-navigation/bottom-tabs" tooltip="https://github.com/react-navigation/react-navigation/tree/6.x/packages/bottom-tabs"/>
+    <hyperlink ref="F19" r:id="rId128" display="链接"/>
+    <hyperlink ref="B21" r:id="rId129" display="@react-navigation/native" tooltip="https://github.com/react-navigation/react-navigation/tree/6.x/packages/native"/>
+    <hyperlink ref="F21" r:id="rId130" display="链接"/>
+    <hyperlink ref="B22" r:id="rId131" display="@react-navigation/stack" tooltip="https://github.com/react-navigation/react-navigation/tree/6.x/packages/stack"/>
+    <hyperlink ref="F22" r:id="rId132" display="链接"/>
+    <hyperlink ref="B113" r:id="rId133" display="recyclerlistview" tooltip="https://github.com/Flipkart/recyclerlistview"/>
+    <hyperlink ref="F113" r:id="rId134" display="链接"/>
+    <hyperlink ref="B120" r:id="rId135" display="rn-placeholder" tooltip="https://github.com/mfrachet/rn-placeholder"/>
+    <hyperlink ref="F120" r:id="rId136" display="链接"/>
+    <hyperlink ref="B121" r:id="rId137" display="styled-components" tooltip="https://github.com/styled-components/styled-components"/>
+    <hyperlink ref="F121" r:id="rId138" display="链接"/>
+    <hyperlink ref="B122" r:id="rId139" display="styled-system" tooltip="https://github.com/react-native-picker/picker"/>
+    <hyperlink ref="F122" r:id="rId140" display="链接"/>
+    <hyperlink ref="B31" r:id="rId141" display="jeanregisser/react-native-slider" tooltip="https://github.com/react-native-oh-library/jeanregisser-react-native-slider"/>
+    <hyperlink ref="F31" r:id="rId142" display="链接"/>
+    <hyperlink ref="B34" r:id="rId80" display="js-beautify" tooltip="https://github.com/beautifier/js-beautify"/>
+    <hyperlink ref="F34" r:id="rId81" display="链接"/>
+    <hyperlink ref="B50" r:id="rId143" display="react-native-base64" tooltip="https://github.com/eranbo/react-native-base64"/>
+    <hyperlink ref="F50" r:id="rId144" display="链接"/>
+    <hyperlink ref="B53" r:id="rId145" display="react-native-check-box" tooltip="https://github.com/crazycodeboy/react-native-check-box"/>
+    <hyperlink ref="F53" r:id="rId146" display="链接"/>
+    <hyperlink ref="B5" r:id="rId147" display="@react-native-community/blur" tooltip="https://github.com/Kureev/react-native-blur"/>
+    <hyperlink ref="E5" r:id="rId148" display="@react-native-oh-tpl/blur Releases" tooltip="https://github.com/react-native-oh-library/react-native-blur/releases"/>
+    <hyperlink ref="F5" r:id="rId149" display="链接"/>
+    <hyperlink ref="B12" r:id="rId150" display="@react-native-community/push-notification-ios" tooltip="https://github.com/react-native-push-notification/ios"/>
+    <hyperlink ref="E12" r:id="rId151" display="@react-native-oh-tpl/push-notification-ios" tooltip="https://github.com/react-native-oh-library/react-native-push-notification-ios/releases"/>
+    <hyperlink ref="F12" r:id="rId152" display="链接"/>
+    <hyperlink ref="B15" r:id="rId153" display="@react-native-cookies/cookies" tooltip="https://github.com/react-native-cookies/cookies"/>
+    <hyperlink ref="E15" r:id="rId154" display="@react-native-oh-tpl/cookies" tooltip="https://github.com/react-native-oh-library/react-native-cookies/releases"/>
+    <hyperlink ref="F15" r:id="rId155" display="链接"/>
+    <hyperlink ref="B55" r:id="rId156" display="react-native-crypto-js" tooltip="https://github.com/imchintan/react-native-crypto-js"/>
+    <hyperlink ref="B73" r:id="rId157" display="react-native-maps" tooltip="https://github.com/react-native-maps/react-native-maps"/>
+    <hyperlink ref="E73" r:id="rId158" display="@react-native-oh-tpl/react-native-maps" tooltip="https://github.com/react-native-maps/react-native-maps/releases"/>
+    <hyperlink ref="F73" r:id="rId159" display="链接"/>
+    <hyperlink ref="B78" r:id="rId160" display="react-native-pdf" tooltip="https://github.com/wonday/react-native-pdf"/>
+    <hyperlink ref="E78" r:id="rId161" display="@react-native-oh-tpl/react-native-pdf" tooltip="https://github.com/react-native-oh-library/react-native-pdf/releases"/>
+    <hyperlink ref="F78" r:id="rId162" display="链接"/>
+    <hyperlink ref="B88" r:id="rId163" display="react-native-redash" tooltip="https://github.com/wcandillon/react-native-redash/"/>
+    <hyperlink ref="F88" r:id="rId164" display="链接"/>
+    <hyperlink ref="B95" r:id="rId165" display="react-native-snap-carousel" tooltip="https://github.com/meliorence/react-native-snap-carousel"/>
+    <hyperlink ref="E95" r:id="rId166" display="@react-native-oh-tpl/react-native-snap-carousel" tooltip="https://github.com/react-native-oh-library/react-native-snap-carousel/releases"/>
+    <hyperlink ref="F95" r:id="rId167" display="链接"/>
+    <hyperlink ref="B103" r:id="rId168" display="react-native-transitiongroup" tooltip="https://github.com/madsleejensen/react-native-transitiongroup"/>
+    <hyperlink ref="E103" r:id="rId169" display="@react-native-oh-tpl/react-native-transitiongroup" tooltip="https://github.com/react-native-oh-library/react-native-transitiongroup/releases"/>
+    <hyperlink ref="F103" r:id="rId170" display="链接"/>
+    <hyperlink ref="B104" r:id="rId171" display="react-native-translucent-modal" tooltip="https://github.com/23mf/react-native-translucent-modal"/>
+    <hyperlink ref="E104" r:id="rId172" display="@react-native-oh-tpl/react-native-translucent-modal" tooltip="https://github.com/react-native-oh-library/react-native-translucent-modal/releases"/>
+    <hyperlink ref="F104" r:id="rId173" display="链接"/>
+    <hyperlink ref="B114" r:id="rId174" display="redux" tooltip="https://github.com/reduxjs/redux"/>
+    <hyperlink ref="F114" r:id="rId175" display="链接"/>
+    <hyperlink ref="B116" r:id="rId176" display="redux-logger" tooltip="https://github.com/LogRocket/redux-logger"/>
+    <hyperlink ref="F116" r:id="rId177" display="链接"/>
+    <hyperlink ref="B117" r:id="rId178" display="redux-persist" tooltip="https://github.com/rt2zz/redux-persist"/>
+    <hyperlink ref="F117" r:id="rId179" display="链接"/>
+    <hyperlink ref="B24" r:id="rId180" display="axios" tooltip="https://github.com/axios/axios"/>
+    <hyperlink ref="F24" r:id="rId181" display="链接"/>
+    <hyperlink ref="B26" r:id="rId182" display="dayJs" tooltip="https://github.com/iamkun/dayjs?tab=readme-ov-file"/>
+    <hyperlink ref="F26" r:id="rId183" display="链接"/>
+    <hyperlink ref="B28" r:id="rId184" display="EventBus" tooltip="https://github.com/krasimir/EventBus"/>
+    <hyperlink ref="F28" r:id="rId185" display="链接"/>
+    <hyperlink ref="B30" r:id="rId186" display="immer" tooltip="https://github.com/immerjs/immer"/>
+    <hyperlink ref="F30" r:id="rId187" display="链接"/>
+    <hyperlink ref="B32" r:id="rId188" display="JsBarCode" tooltip="https://github.com/lindell/JsBarcode"/>
+    <hyperlink ref="F32" r:id="rId189" display="链接"/>
+    <hyperlink ref="B39" r:id="rId190" display="Moment" tooltip="https://github.com/moment/moment"/>
+    <hyperlink ref="F39" r:id="rId191" display="链接"/>
+    <hyperlink ref="B42" r:id="rId192" display="qrcode-generator" tooltip="https://github.com/kazuhikoarase/qrcode-generator"/>
+    <hyperlink ref="F42" r:id="rId193" display="链接"/>
+    <hyperlink ref="B43" r:id="rId194" display="react-ahooks" tooltip="https://github.com/alibaba/hooks"/>
+    <hyperlink ref="F43" r:id="rId195" display="链接"/>
+    <hyperlink ref="B45" r:id="rId196" display="react-lifecycles-compat" tooltip="https://github.com/reactjs/react-lifecycles-compat"/>
+    <hyperlink ref="F45" r:id="rId197" display="链接"/>
+    <hyperlink ref="B47" r:id="rId198" display="react-native-animate-number" tooltip="https://github.com/wkh237/react-native-animate-number"/>
+    <hyperlink ref="F47" r:id="rId199" display="链接"/>
+    <hyperlink ref="B51" r:id="rId200" display="react-native-blob-util" tooltip="https://github.com/react-native-oh-library/react-native-blob-util"/>
+    <hyperlink ref="E51" r:id="rId201" display="@react-native-oh-tpl/react-native-blob-util" tooltip="https://github.com/react-native-oh-library/react-native-blob-util/releases"/>
+    <hyperlink ref="F51" r:id="rId202" display="链接"/>
+    <hyperlink ref="B52" r:id="rId203" display="react-native-canvas" tooltip="https://github.com/iddan/react-native-canvas"/>
+    <hyperlink ref="F52" r:id="rId204" display="链接"/>
+    <hyperlink ref="B54" r:id="rId205" display="react-native-confirmation-code-field" tooltip="https://github.com/retyui/react-native-confirmation-code-field"/>
+    <hyperlink ref="F54" r:id="rId206" display="链接"/>
+    <hyperlink ref="B58" r:id="rId207" display="react-native-drawer-layout-polyfill" tooltip="https://github.com/rnc-archive/react-native-drawer-layout-polyfill"/>
+    <hyperlink ref="F58" r:id="rId208" display="链接"/>
+    <hyperlink ref="B59" r:id="rId209" display="react-native-echarts-pro" tooltip="https://github.com/supervons/react-native-echarts-pro"/>
+    <hyperlink ref="F59" r:id="rId210" display="链接"/>
+    <hyperlink ref="B62" r:id="rId211" display="react-native-fit-Image" tooltip="https://github.com/huiseoul/react-native-fit-image"/>
+    <hyperlink ref="E62" r:id="rId212" display="@react-native-oh-tpl/react-native-fit-Image" tooltip="https://github.com/huiseoul/react-native-fit-image/releases"/>
+    <hyperlink ref="F62" r:id="rId213" display="链接"/>
+    <hyperlink ref="B65" r:id="rId214" display="react-native-image-editor" tooltip="https://github.com/react-native-oh-library/react-native-image-editor"/>
+    <hyperlink ref="E65" r:id="rId215" display="@react-native-oh-tpl/react-native-image-editor" tooltip="https://github.com/react-native-oh-library/react-native-image-editor/releases"/>
+    <hyperlink ref="F65" r:id="rId216" display="链接"/>
+    <hyperlink ref="B67" r:id="rId217" display="react-native-image-viewer" tooltip="https://github.com/react-native-oh-library/react-native-image-viewer"/>
+    <hyperlink ref="E67" r:id="rId218" display="react-native-image-viewer" tooltip="https://github.com/react-native-oh-library/react-native-image-viewer/releases"/>
+    <hyperlink ref="F67" r:id="rId219" display="链接"/>
+    <hyperlink ref="B69" r:id="rId220" display="react-native-image-zoom" tooltip="https://github.com/react-native-oh-library/react-native-image-zoom"/>
+    <hyperlink ref="E69" r:id="rId221" display="@react-native-oh-tpl/react-native-image-zoom" tooltip="https://github.com/react-native-oh-library/react-native-image-zoom/releases"/>
+    <hyperlink ref="F69" r:id="rId222" display="链接"/>
+    <hyperlink ref="B70" r:id="rId223" display="react-native-intersection-observer" tooltip="https://github.com/react-native-oh-library/react-native-intersection-observer"/>
+    <hyperlink ref="E70" r:id="rId224" display="@react-native-oh-tpl/react-native-intersection-observer" tooltip="https://github.com/react-native-oh-library/react-native-intersection-observer/releases"/>
+    <hyperlink ref="F70" r:id="rId225" display="链接"/>
+    <hyperlink ref="B68" r:id="rId226" display="react-native-image-viewing" tooltip="https://github.com/react-native-oh-library/react-native-image-viewing"/>
+    <hyperlink ref="E68" r:id="rId227" display="@react-native-oh-tpl/react-native-image-viewing" tooltip="https://github.com/react-native-oh-library/react-native-image-viewing/releases"/>
+    <hyperlink ref="F68" r:id="rId228" display="链接"/>
+    <hyperlink ref="B74" r:id="rId229" display="react-native-markdown-display" tooltip="https://github.com/react-native-oh-library/react-native-markdown-display/tree/sig"/>
+    <hyperlink ref="E74" r:id="rId230" display="@react-native-oh-tpl/react-native-markdown-display" tooltip="https://github.com/react-native-oh-library/react-native-markdown-display/releases"/>
+    <hyperlink ref="F74" r:id="rId231" display="链接"/>
+    <hyperlink ref="B75" r:id="rId232" display="react-native-marquee" tooltip="https://github.com/react-native-oh-library/react-native-marquee"/>
+    <hyperlink ref="E75" r:id="rId233" display="@react-native-oh-tpl/react-native-marquee" tooltip="https://github.com/react-native-oh-library/react-native-marquee/releases"/>
+    <hyperlink ref="F75" r:id="rId234" display="链接"/>
+    <hyperlink ref="B80" r:id="rId235" display="react-native-popover-view" tooltip="https://github.com/react-native-oh-library/react-native-popover-view"/>
+    <hyperlink ref="E80" r:id="rId236" display="@react-native-oh-tpl/react-native-popover-view" tooltip="https://github.com/react-native-oh-library/react-native-popover-view/releases"/>
+    <hyperlink ref="F80" r:id="rId237" display="链接"/>
+    <hyperlink ref="B81" r:id="rId238" display="react-native-popup-menu" tooltip="https://github.com/instea/react-native-popup-menu"/>
+    <hyperlink ref="F81" r:id="rId239" display="链接"/>
+    <hyperlink ref="B83" r:id="rId240" display="react-native-pull" tooltip="https://github.com/react-native-oh-library/react-native-pull"/>
+    <hyperlink ref="E83" r:id="rId241" display="@react-native-oh-tpl/react-native-pull" tooltip="https://github.com/react-native-oh-library/react-native-pull/releases"/>
+    <hyperlink ref="F83" r:id="rId242" display="链接"/>
+    <hyperlink ref="B87" r:id="rId243" display="react-native-reanimated-table" tooltip="https://github.com/dohooo/react-native-reanimated-table"/>
+    <hyperlink ref="F87" r:id="rId244" display="链接"/>
+    <hyperlink ref="B92" r:id="rId245" display="react-native-scrollable-tab-view" tooltip="https://github.com/react-native-oh-library/react-native-scrollable-tab-view"/>
+    <hyperlink ref="F92" r:id="rId246" display="链接"/>
+    <hyperlink ref="B97" r:id="rId247" display="react-native-stickyheader" tooltip="https://github.com/react-native-oh-library/react-native-stickyheader"/>
+    <hyperlink ref="E97" r:id="rId248" display="@react-native-oh-tpl/react-native-stickyheader" tooltip="https://github.com/react-native-oh-library/react-native-stickyheader/releases"/>
+    <hyperlink ref="F97" r:id="rId249" display="链接"/>
+    <hyperlink ref="B99" r:id="rId207" display="react-native-swipe-list-view" tooltip="https://github.com/rnc-archive/react-native-drawer-layout-polyfill"/>
+    <hyperlink ref="F99" r:id="rId250" display="链接"/>
+    <hyperlink ref="B100" r:id="rId251" display="react-native-swiper" tooltip="https://github.com/leecade/react-native-swiper"/>
+    <hyperlink ref="F100" r:id="rId252" display="链接"/>
+    <hyperlink ref="B109" r:id="rId253" display="react-native-worklets-core" tooltip="https://github.com/react-native-oh-library/react-native-worklets-core"/>
+    <hyperlink ref="E109" r:id="rId254" display="@react-native-oh-tpl/react-native-worklets-core" tooltip="https://github.com/react-native-oh-library/react-native-worklets-core/releases"/>
+    <hyperlink ref="F109" r:id="rId255" display="链接"/>
+    <hyperlink ref="B112" r:id="rId256" display="react-use" tooltip="https://github.com/zenghongtu/react-use"/>
+    <hyperlink ref="F112" r:id="rId257" display="链接"/>
+    <hyperlink ref="B119" r:id="rId258" display="redux-toolkit" tooltip="https://github.com/reduxjs/redux-toolkit"/>
+    <hyperlink ref="F119" r:id="rId259" display="链接"/>
+    <hyperlink ref="B102" r:id="rId260" display="react-native-text-size" tooltip="https://github.com/aMarCruz/react-native-text-size"/>
+    <hyperlink ref="E102" r:id="rId261" display="@react-native-oh-tpl/react-native-text-size" tooltip="https://github.com/react-native-oh-library/react-native-text-size/releases"/>
+    <hyperlink ref="F102" r:id="rId262" display="链接"/>
+    <hyperlink ref="B111" r:id="rId263" display="react-router-dom" tooltip="https://github.com/remix-run/react-router"/>
+    <hyperlink ref="F111" r:id="rId264" display="链接"/>
+    <hyperlink ref="B115" r:id="rId265" display="redux-actions" tooltip="https://github.com/redux-utilities/redux-actions"/>
+    <hyperlink ref="F115" r:id="rId266" display="链接"/>
+    <hyperlink ref="B118" r:id="rId267" display="redux-thunk" tooltip="https://github.com/reduxjs/redux-thunk"/>
+    <hyperlink ref="F118" r:id="rId268" display="链接"/>
+    <hyperlink ref="B48" r:id="rId269" display="react-native-aria" tooltip="https://github.com/gluestack/react-native-aria/"/>
+    <hyperlink ref="F48" r:id="rId270" display="链接"/>
+    <hyperlink ref="B82" r:id="rId271" display="react-native-progress" tooltip="https://github.com/oblador/react-native-progress"/>
+    <hyperlink ref="E82" r:id="rId272" display="@react-native-oh-tpl/react-native-progress" tooltip="https://github.com/react-native-oh-library/react-native-progress/releases"/>
+    <hyperlink ref="F82" r:id="rId273" display="链接"/>
+    <hyperlink ref="B63" r:id="rId274" display="react-native-fs" tooltip="https://github.com/itinance/react-native-fs"/>
+    <hyperlink ref="E63" r:id="rId275" display="@react-native-oh-tpl/react-native-fs" tooltip="https://github.com/react-native-oh-library/react-native-fs/releases"/>
+    <hyperlink ref="F63" r:id="rId276" display="链接"/>
+    <hyperlink ref="B71" r:id="rId277" display="react-native-keyboard-aware-scroll-view" tooltip="https://github.com/APSL/react-native-keyboard-aware-scroll-view"/>
+    <hyperlink ref="E71" r:id="rId278" display="@react-native-oh-tpl/react-native-keyboard-aware-scroll-view" tooltip="https://github.com/react-native-oh-library/react-native-keyboard-aware-scroll-view/releases"/>
+    <hyperlink ref="F71" r:id="rId279" display="链接"/>
+    <hyperlink ref="B79" r:id="rId280" display="react-native-permissions" tooltip="https://github.com/zoontek/react-native-permissions"/>
+    <hyperlink ref="E79" r:id="rId281" display="@react-native-oh-tpl/react-native-permissions" tooltip="https://github.com/react-native-oh-library/react-native-permissions/releases"/>
+    <hyperlink ref="F79" r:id="rId282" display="链接"/>
+    <hyperlink ref="B57" r:id="rId283" display="react-native-drag-sort" tooltip="https://github.com/mochixuan/react-native-drag-sort"/>
+    <hyperlink ref="F57" r:id="rId284" display="链接"/>
+    <hyperlink ref="B96" r:id="rId285" display="react-native-sound" tooltip="https://github.com/zmxv/react-native-sound"/>
+    <hyperlink ref="E96" r:id="rId286" display="@react-native-oh-tpl/react-native-sound" tooltip="https://github.com/react-native-oh-library/react-native-sound/releases"/>
+    <hyperlink ref="F96" r:id="rId287" display="链接"/>
+    <hyperlink ref="B86" r:id="rId288" display="react-native-reanimated-carousel" tooltip="https://github.com/dohooo/react-native-reanimated-carousel"/>
+    <hyperlink ref="F86" r:id="rId289" display="链接"/>
+    <hyperlink ref="B14" r:id="rId290" display="@react-native-community/toolbar-android" tooltip="https://github.com/react-native-toolbar-android/toolbar-android"/>
+    <hyperlink ref="E14" r:id="rId291" display="@react-native-oh-tpl/toolbar-android" tooltip="https://github.com/react-native-oh-library/toolbar-android/releases"/>
+    <hyperlink ref="F14" r:id="rId292" display="链接"/>
+    <hyperlink ref="B110" r:id="rId293" display="react-redux" tooltip="https://github.com/reduxjs/react-redux"/>
+    <hyperlink ref="F110" r:id="rId294" display="链接"/>
+    <hyperlink ref="B76" r:id="rId295" display="react-native-MJRefresh" tooltip="https://github.com/react-native-studio/react-native-MJRefresh"/>
+    <hyperlink ref="E76" r:id="rId296" display="@react-native-oh-tpl/react-native-mjrefresh" tooltip="https://github.com/react-native-oh-library/react-native-MJRefresh/releases"/>
+    <hyperlink ref="E92" r:id="rId297" display="@react-native-oh-tpl/react-native-scrollable-tab-view" tooltip="https://github.com/react-native-oh-library/react-native-scrollable-tab-view/releases"/>
+    <hyperlink ref="F55" r:id="rId298" display="链接"/>
+    <hyperlink ref="F76" r:id="rId299" display="链接"/>
+    <hyperlink ref="F123" r:id="rId300" display="链接"/>
+    <hyperlink ref="F124" r:id="rId301" display="链接"/>
+    <hyperlink ref="E124" r:id="rId302" display="@react-native-oh-tpl/react-native-sortable-list"/>
+    <hyperlink ref="B124" r:id="rId303" display="react-native-sortable-list"/>
+    <hyperlink ref="B123" r:id="rId304" display="react-native-sensors"/>
+    <hyperlink ref="E123" r:id="rId305" display="@react-native-oh-tpl/react-native-sensors"/>
+    <hyperlink ref="B126" r:id="rId306" display="react-native-image-sequence-2"/>
+    <hyperlink ref="E126" r:id="rId307" display="@react-native-oh-tpl/react-native-image-sequence-2"/>
+    <hyperlink ref="F126" r:id="rId308" display="链接"/>
+    <hyperlink ref="B127" r:id="rId309" display="react-native-feather"/>
+    <hyperlink ref="F127" r:id="rId310" display="链接"/>
+    <hyperlink ref="B125" r:id="rId311" display="react-native-easy-toast"/>
+    <hyperlink ref="F125" r:id="rId312" display="链接"/>
+    <hyperlink ref="B128" r:id="rId313" display="@react-navigation/native-stack"/>
+    <hyperlink ref="E128" r:id="rId314" display="@react-native-oh-tpl/native-stack"/>
+    <hyperlink ref="F128" r:id="rId315" display="链接"/>
+    <hyperlink ref="B129" r:id="rId316" display="react-native-waterfall-flow"/>
+    <hyperlink ref="F129" r:id="rId317" display="链接"/>
+    <hyperlink ref="B130" r:id="rId318" display="react-native-vconsole"/>
+    <hyperlink ref="F130" r:id="rId319" display="链接"/>
+    <hyperlink ref="B131" r:id="rId320" display="better-banner"/>
+    <hyperlink ref="F131" r:id="rId321" display="链接"/>
+    <hyperlink ref="B132" r:id="rId322" display="react-native-ezswiper"/>
+    <hyperlink ref="F132" r:id="rId323" display="链接"/>
+    <hyperlink ref="B133" r:id="rId324" display="react-native-image-header-scroll-view"/>
+    <hyperlink ref="F133" r:id="rId325" display="链接"/>
+    <hyperlink ref="B134" r:id="rId326" display="react-native-linear-gradient-text"/>
+    <hyperlink ref="F134" r:id="rId327" display="链接"/>
+    <hyperlink ref="B135" r:id="rId328" display="react-native-marquee-ab"/>
+    <hyperlink ref="F135" r:id="rId329" display="链接"/>
+    <hyperlink ref="B136" r:id="rId330" display="react-native-reconnecting-websocket"/>
+    <hyperlink ref="F136" r:id="rId331" display="链接"/>
+    <hyperlink ref="B137" r:id="rId332" display="react-native-json-tree"/>
+    <hyperlink ref="F137" r:id="rId333" display="链接"/>
+    <hyperlink ref="B138" r:id="rId334" display="react-native-image-gallery"/>
+    <hyperlink ref="F138" r:id="rId335" display="链接"/>
+    <hyperlink ref="E138" r:id="rId336" display="@react-native-oh-tpl/react-native-image-gallery"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
docs: [Issues: #IA6F3D] 新增react-native-image-base64指导文档
</commit_message>
<xml_diff>
--- a/Menu.xlsx
+++ b/Menu.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375"/>
+    <workbookView windowWidth="28800" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="345">
   <si>
     <t>序号</t>
   </si>
@@ -983,6 +983,15 @@
     <t>@react-native-oh-tpl/native-stack</t>
   </si>
   <si>
+    <t>react-native-clippath</t>
+  </si>
+  <si>
+    <t>1.1.8</t>
+  </si>
+  <si>
+    <t>@react-native-oh-tpl/react-native-clippath</t>
+  </si>
+  <si>
     <t>react-native-waterfall-flow</t>
   </si>
   <si>
@@ -1041,6 +1050,21 @@
   </si>
   <si>
     <t>@react-native-oh-tpl/react-native-image-gallery</t>
+  </si>
+  <si>
+    <t>react-native-image-crop-picker</t>
+  </si>
+  <si>
+    <t>0.40.3</t>
+  </si>
+  <si>
+    <t>@react-native-oh-tpl/react-native-image-crop-picker</t>
+  </si>
+  <si>
+    <t>react-native-image-image-base64</t>
+  </si>
+  <si>
+    <t>0.1.3</t>
   </si>
 </sst>
 </file>
@@ -1053,7 +1077,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1091,12 +1115,6 @@
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1583,128 +1601,128 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1721,18 +1739,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2260,10 +2266,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F139"/>
+  <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="G138" sqref="G138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -4718,324 +4724,389 @@
       <c r="A123" s="3">
         <v>122</v>
       </c>
-      <c r="B123" s="6" t="s">
+      <c r="B123" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="C123" s="4" t="s">
+      <c r="C123" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="D123" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E123" s="6" t="s">
+      <c r="D123" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E123" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="F123" s="4" t="s">
+      <c r="F123" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="124" ht="14.25" spans="1:6">
-      <c r="A124" s="1">
+      <c r="A124" s="3">
         <v>123</v>
       </c>
-      <c r="B124" s="6" t="s">
+      <c r="B124" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="C124" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="D124" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E124" s="7" t="s">
+      <c r="D124" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E124" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="F124" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6">
-      <c r="A125" s="1">
+      <c r="F124" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125" ht="14.25" spans="1:6">
+      <c r="A125" s="3">
         <v>124</v>
       </c>
-      <c r="B125" s="8" t="s">
+      <c r="B125" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C125" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="D125" s="1" t="s">
+      <c r="D125" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E125" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F125" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6">
-      <c r="A126" s="1">
+      <c r="F125" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="126" ht="14.25" spans="1:6">
+      <c r="A126" s="3">
         <v>125</v>
       </c>
-      <c r="B126" s="8" t="s">
+      <c r="B126" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="C126" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="D126" s="1" t="s">
+      <c r="D126" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E126" s="8" t="s">
+      <c r="E126" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="F126" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6">
-      <c r="A127" s="1">
+      <c r="F126" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" ht="14.25" spans="1:6">
+      <c r="A127" s="3">
         <v>126</v>
       </c>
-      <c r="B127" s="8" t="s">
+      <c r="B127" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="C127" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="D127" s="1" t="s">
+      <c r="D127" s="3" t="s">
         <v>59</v>
       </c>
       <c r="E127" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F127" s="7" t="s">
+      <c r="F127" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="128" ht="14.25" spans="1:6">
-      <c r="A128" s="1">
+      <c r="A128" s="3">
         <v>127</v>
       </c>
-      <c r="B128" s="8" t="s">
+      <c r="B128" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="C128" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="D128" s="9" t="s">
+      <c r="D128" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="E128" s="7" t="s">
+      <c r="E128" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="F128" s="7" t="s">
+      <c r="F128" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="129" ht="14.25" spans="1:6">
-      <c r="A129" s="1">
+      <c r="A129" s="3">
         <v>128</v>
       </c>
-      <c r="B129" s="8" t="s">
+      <c r="B129" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="C129" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="D129" s="9" t="s">
+      <c r="D129" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E129" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="F129" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130" ht="14.25" spans="1:6">
+      <c r="A130" s="3">
+        <v>129</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="D130" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="E129" s="9" t="s">
+      <c r="E130" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="F129" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="130" ht="14.25" spans="1:6">
-      <c r="A130" s="1">
-        <v>129</v>
-      </c>
-      <c r="B130" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="D130" s="9" t="s">
+      <c r="F130" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" ht="14.25" spans="1:6">
+      <c r="A131" s="3">
+        <v>130</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="D131" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="E130" s="9" t="s">
+      <c r="E131" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="F130" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="131" ht="14.25" spans="1:6">
-      <c r="A131" s="1">
-        <v>130</v>
-      </c>
-      <c r="B131" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="D131" s="9" t="s">
+      <c r="F131" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" ht="14.25" spans="1:6">
+      <c r="A132" s="3">
+        <v>131</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="D132" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="E131" s="9" t="s">
+      <c r="E132" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="F131" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="132" ht="14.25" spans="1:6">
-      <c r="A132" s="1">
-        <v>131</v>
-      </c>
-      <c r="B132" s="8" t="s">
-        <v>323</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="D132" s="9" t="s">
+      <c r="F132" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" ht="14.25" spans="1:6">
+      <c r="A133" s="3">
+        <v>132</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="D133" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="E132" s="9" t="s">
+      <c r="E133" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="F132" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="133" ht="14.25" spans="1:6">
-      <c r="A133" s="1">
-        <v>132</v>
-      </c>
-      <c r="B133" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="D133" s="9" t="s">
+      <c r="F133" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" ht="14.25" spans="1:6">
+      <c r="A134" s="3">
+        <v>133</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D134" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="E133" s="9" t="s">
+      <c r="E134" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="F133" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="134" ht="14.25" spans="1:6">
-      <c r="A134" s="1">
-        <v>133</v>
-      </c>
-      <c r="B134" s="7" t="s">
+      <c r="F134" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="135" ht="14.25" spans="1:6">
+      <c r="A135" s="3">
+        <v>134</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="E135" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="F135" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" ht="27.75" spans="1:6">
+      <c r="A136" s="3">
+        <v>135</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="E136" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="F136" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="137" ht="14.25" spans="1:6">
+      <c r="A137" s="3">
+        <v>136</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="E137" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="F137" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="138" ht="14.25" spans="1:6">
+      <c r="A138" s="3">
+        <v>137</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C138" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="C134" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D134" s="9" t="s">
+      <c r="D138" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="E134" s="9" t="s">
+      <c r="E138" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="F134" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="135" ht="14.25" spans="1:6">
-      <c r="A135" s="1">
-        <v>134</v>
-      </c>
-      <c r="B135" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="D135" s="9" t="s">
+      <c r="F138" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" ht="14.25" spans="1:6">
+      <c r="A139" s="3">
+        <v>138</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="D139" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="E135" s="9" t="s">
+      <c r="E139" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="F139" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" ht="14.25" spans="1:6">
+      <c r="A140" s="3">
+        <v>139</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="D140" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E140" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="F140" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="141" ht="14.25" spans="1:6">
+      <c r="A141" s="3">
+        <v>140</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="D141" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="F135" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="136" ht="14.25" spans="1:6">
-      <c r="A136" s="1">
-        <v>135</v>
-      </c>
-      <c r="B136" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="D136" s="9" t="s">
+      <c r="E141" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="E136" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="F136" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="137" ht="14.25" spans="1:6">
-      <c r="A137" s="1">
-        <v>136</v>
-      </c>
-      <c r="B137" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="D137" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="E137" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="F137" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="138" ht="14.25" spans="1:6">
-      <c r="A138" s="1">
-        <v>137</v>
-      </c>
-      <c r="B138" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="D138" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="E138" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F138" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="139" ht="14.25" spans="2:2">
-      <c r="B139" s="9"/>
+      <c r="F141" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142" ht="14.25" spans="1:6">
+      <c r="A142" s="3"/>
+      <c r="B142" s="3"/>
+      <c r="C142" s="3"/>
+      <c r="D142" s="3"/>
+      <c r="E142" s="5"/>
+      <c r="F142" s="3"/>
     </row>
   </sheetData>
   <sortState ref="A2:F122">
@@ -5361,27 +5432,35 @@
     <hyperlink ref="B128" r:id="rId313" display="@react-navigation/native-stack"/>
     <hyperlink ref="E128" r:id="rId314" display="@react-native-oh-tpl/native-stack"/>
     <hyperlink ref="F128" r:id="rId315" display="链接"/>
-    <hyperlink ref="B129" r:id="rId316" display="react-native-waterfall-flow"/>
-    <hyperlink ref="F129" r:id="rId317" display="链接"/>
-    <hyperlink ref="B130" r:id="rId318" display="react-native-vconsole"/>
-    <hyperlink ref="F130" r:id="rId319" display="链接"/>
-    <hyperlink ref="B131" r:id="rId320" display="better-banner"/>
-    <hyperlink ref="F131" r:id="rId321" display="链接"/>
-    <hyperlink ref="B132" r:id="rId322" display="react-native-ezswiper"/>
-    <hyperlink ref="F132" r:id="rId323" display="链接"/>
-    <hyperlink ref="B133" r:id="rId324" display="react-native-image-header-scroll-view"/>
-    <hyperlink ref="F133" r:id="rId325" display="链接"/>
-    <hyperlink ref="B134" r:id="rId326" display="react-native-linear-gradient-text"/>
-    <hyperlink ref="F134" r:id="rId327" display="链接"/>
-    <hyperlink ref="B135" r:id="rId328" display="react-native-marquee-ab"/>
-    <hyperlink ref="F135" r:id="rId329" display="链接"/>
-    <hyperlink ref="B136" r:id="rId330" display="react-native-reconnecting-websocket"/>
-    <hyperlink ref="F136" r:id="rId331" display="链接"/>
-    <hyperlink ref="B137" r:id="rId332" display="react-native-json-tree"/>
-    <hyperlink ref="F137" r:id="rId333" display="链接"/>
-    <hyperlink ref="B138" r:id="rId334" display="react-native-image-gallery"/>
-    <hyperlink ref="F138" r:id="rId335" display="链接"/>
-    <hyperlink ref="E138" r:id="rId336" display="@react-native-oh-tpl/react-native-image-gallery"/>
+    <hyperlink ref="B130" r:id="rId316" display="react-native-waterfall-flow"/>
+    <hyperlink ref="F130" r:id="rId317" display="链接"/>
+    <hyperlink ref="B131" r:id="rId318" display="react-native-vconsole"/>
+    <hyperlink ref="F131" r:id="rId319" display="链接"/>
+    <hyperlink ref="B132" r:id="rId320" display="better-banner"/>
+    <hyperlink ref="F132" r:id="rId321" display="链接"/>
+    <hyperlink ref="B133" r:id="rId322" display="react-native-ezswiper"/>
+    <hyperlink ref="F133" r:id="rId323" display="链接"/>
+    <hyperlink ref="B134" r:id="rId324" display="react-native-image-header-scroll-view"/>
+    <hyperlink ref="F134" r:id="rId325" display="链接"/>
+    <hyperlink ref="B135" r:id="rId326" display="react-native-linear-gradient-text"/>
+    <hyperlink ref="F135" r:id="rId327" display="链接"/>
+    <hyperlink ref="B136" r:id="rId328" display="react-native-marquee-ab"/>
+    <hyperlink ref="F136" r:id="rId329" display="链接"/>
+    <hyperlink ref="B137" r:id="rId330" display="react-native-reconnecting-websocket"/>
+    <hyperlink ref="F137" r:id="rId331" display="链接"/>
+    <hyperlink ref="B138" r:id="rId332" display="react-native-json-tree"/>
+    <hyperlink ref="F138" r:id="rId333" display="链接"/>
+    <hyperlink ref="B139" r:id="rId334" display="react-native-image-gallery"/>
+    <hyperlink ref="F139" r:id="rId335" display="链接"/>
+    <hyperlink ref="E139" r:id="rId336" display="@react-native-oh-tpl/react-native-image-gallery"/>
+    <hyperlink ref="B129" r:id="rId337" display="react-native-clippath"/>
+    <hyperlink ref="E129" r:id="rId338" display="@react-native-oh-tpl/react-native-clippath"/>
+    <hyperlink ref="F129" r:id="rId339" display="链接"/>
+    <hyperlink ref="B140" r:id="rId340" display="react-native-image-crop-picker"/>
+    <hyperlink ref="B141" r:id="rId341" display="react-native-image-image-base64"/>
+    <hyperlink ref="E140" r:id="rId342" display="@react-native-oh-tpl/react-native-image-crop-picker"/>
+    <hyperlink ref="F140" r:id="rId343" display="链接"/>
+    <hyperlink ref="F141" r:id="rId344" display="链接"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>